<commit_message>
algumas modificações nas visualizações
</commit_message>
<xml_diff>
--- a/doc/resultados_beta.xlsx
+++ b/doc/resultados_beta.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,7 @@
         <v>45288</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0126182965299686</v>
+        <v>0.00888647080159588</v>
       </c>
       <c r="C2" t="n">
         <v>-6.706708198578326e-05</v>
@@ -468,7 +468,7 @@
         <v>45287</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.002492211838006186</v>
+        <v>-0.001438072982203997</v>
       </c>
       <c r="C3" t="n">
         <v>0.004950087244351531</v>
@@ -479,7 +479,7 @@
         <v>45286</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.006870705808869504</v>
+        <v>-0.005940594059405946</v>
       </c>
       <c r="C4" t="n">
         <v>0.005875573433368642</v>
@@ -490,7 +490,7 @@
         <v>45282</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.010062893081761</v>
+        <v>-0.005070626584570803</v>
       </c>
       <c r="C5" t="n">
         <v>0.00431980148583011</v>
@@ -501,7 +501,7 @@
         <v>45281</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.01556543837357061</v>
+        <v>-0.008918820531488847</v>
       </c>
       <c r="C6" t="n">
         <v>0.01053484602917343</v>
@@ -512,7 +512,7 @@
         <v>45280</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.006776379477250627</v>
+        <v>-0.01010101010101017</v>
       </c>
       <c r="C7" t="n">
         <v>-0.007940781639881433</v>
@@ -523,7 +523,7 @@
         <v>45279</v>
       </c>
       <c r="B8" t="n">
-        <v>0.01039636127355426</v>
+        <v>-0.01725417439703159</v>
       </c>
       <c r="C8" t="n">
         <v>0.005851209911202027</v>
@@ -534,7 +534,7 @@
         <v>45278</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.0006430868167203174</v>
+        <v>-0.007929016424391144</v>
       </c>
       <c r="C9" t="n">
         <v>0.006812752982019665</v>
@@ -545,7 +545,7 @@
         <v>45275</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.004826254826254761</v>
+        <v>0.001522359657469163</v>
       </c>
       <c r="C10" t="n">
         <v>-0.004929609758334452</v>
@@ -556,7 +556,7 @@
         <v>45274</v>
       </c>
       <c r="B11" t="n">
-        <v>0.004526349822179032</v>
+        <v>-0.004180125403762225</v>
       </c>
       <c r="C11" t="n">
         <v>0.01063607924921794</v>
@@ -567,7 +567,7 @@
         <v>45273</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.008368200836820106</v>
+        <v>-0.010684983781721</v>
       </c>
       <c r="C12" t="n">
         <v>0.02422410860501722</v>
@@ -578,7 +578,7 @@
         <v>45272</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.02953586497890293</v>
+        <v>-0.01716489874638383</v>
       </c>
       <c r="C13" t="n">
         <v>-0.004042043556367947</v>
@@ -589,7 +589,7 @@
         <v>45271</v>
       </c>
       <c r="B14" t="n">
-        <v>0.005016722408026864</v>
+        <v>0.008634222919937207</v>
       </c>
       <c r="C14" t="n">
         <v>-0.001400538184336053</v>
@@ -600,7 +600,7 @@
         <v>45268</v>
       </c>
       <c r="B15" t="n">
-        <v>0.00698835274542442</v>
+        <v>-0.01225680933852136</v>
       </c>
       <c r="C15" t="n">
         <v>0.008602491865725037</v>
@@ -611,7 +611,7 @@
         <v>45267</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.01255783212161277</v>
+        <v>-0.02028757140043336</v>
       </c>
       <c r="C16" t="n">
         <v>0.003080646060036774</v>
@@ -622,7 +622,7 @@
         <v>45266</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.009705488621151281</v>
+        <v>0.003216726980297402</v>
       </c>
       <c r="C17" t="n">
         <v>-0.01008644397689573</v>
@@ -633,7 +633,7 @@
         <v>45265</v>
       </c>
       <c r="B18" t="n">
-        <v>0.008786752281176202</v>
+        <v>0.007414829659318833</v>
       </c>
       <c r="C18" t="n">
         <v>0.0007886248748059099</v>
@@ -644,7 +644,7 @@
         <v>45264</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.008040201005025227</v>
+        <v>0.006564551422319376</v>
       </c>
       <c r="C19" t="n">
         <v>-0.01014808396368549</v>
@@ -655,7 +655,7 @@
         <v>45261</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.001350894967916183</v>
+        <v>-0.0005928853754940677</v>
       </c>
       <c r="C20" t="n">
         <v>0.006062938326095058</v>
@@ -666,7 +666,7 @@
         <v>45260</v>
       </c>
       <c r="B21" t="n">
-        <v>0.002367264119039536</v>
+        <v>0.03915364840814717</v>
       </c>
       <c r="C21" t="n">
         <v>0.00975408601042016</v>
@@ -677,7 +677,7 @@
         <v>45259</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.01518218623481782</v>
+        <v>0.008753568030447134</v>
       </c>
       <c r="C22" t="n">
         <v>-0.003453508037111419</v>
@@ -688,7 +688,7 @@
         <v>45258</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.006851661527920605</v>
+        <v>-0.01660064138841721</v>
       </c>
       <c r="C23" t="n">
         <v>0.006802829340483596</v>
@@ -699,7 +699,7 @@
         <v>45257</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.009658502932045399</v>
+        <v>0.007481296758104827</v>
       </c>
       <c r="C24" t="n">
         <v>0.001123130107852255</v>
@@ -710,7 +710,7 @@
         <v>45254</v>
       </c>
       <c r="B25" t="n">
-        <v>0.002438174851967956</v>
+        <v>-0.005331302361005319</v>
       </c>
       <c r="C25" t="n">
         <v>-0.008169005182657063</v>
@@ -721,7 +721,7 @@
         <v>45253</v>
       </c>
       <c r="B26" t="n">
-        <v>0.005559416261292638</v>
+        <v>0.00631699846860645</v>
       </c>
       <c r="C26" t="n">
         <v>0.004292458444083103</v>
@@ -732,7 +732,7 @@
         <v>45252</v>
       </c>
       <c r="B27" t="n">
-        <v>0.001382170006910766</v>
+        <v>-0.0068480121742438</v>
       </c>
       <c r="C27" t="n">
         <v>0.003407453406259142</v>
@@ -743,7 +743,7 @@
         <v>45251</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.006211180124223614</v>
+        <v>-0.008427504309519218</v>
       </c>
       <c r="C28" t="n">
         <v>-0.003870097942027861</v>
@@ -754,7 +754,7 @@
         <v>45250</v>
       </c>
       <c r="B29" t="n">
-        <v>0.00173611111111116</v>
+        <v>-0.00154529650376678</v>
       </c>
       <c r="C29" t="n">
         <v>0.008259903088068343</v>
@@ -765,7 +765,7 @@
         <v>45247</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.009705372616984453</v>
+        <v>0.0007738440704196936</v>
       </c>
       <c r="C30" t="n">
         <v>0.003901232982275848</v>
@@ -776,7 +776,7 @@
         <v>45246</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.004550227511375571</v>
+        <v>0.008699014111734016</v>
       </c>
       <c r="C31" t="n">
         <v>0.01011935651271401</v>
@@ -787,7 +787,7 @@
         <v>45244</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.01582278481012667</v>
+        <v>-0.01686469911843624</v>
       </c>
       <c r="C32" t="n">
         <v>0.02452316076294281</v>
@@ -798,7 +798,7 @@
         <v>45243</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.01500535905680589</v>
+        <v>0.03040935672514622</v>
       </c>
       <c r="C33" t="n">
         <v>-0.002155243874133794</v>
@@ -809,7 +809,7 @@
         <v>45240</v>
       </c>
       <c r="B34" t="n">
-        <v>0.006891548784911272</v>
+        <v>0.01002648505486192</v>
       </c>
       <c r="C34" t="n">
         <v>0.01364568278829026</v>
@@ -820,7 +820,7 @@
         <v>45239</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.01188760806916433</v>
+        <v>-0.02210151713804087</v>
       </c>
       <c r="C35" t="n">
         <v>-0.0007304847227936895</v>
@@ -831,7 +831,7 @@
         <v>45238</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.00437477214728399</v>
+        <v>0.0009576709442635778</v>
       </c>
       <c r="C36" t="n">
         <v>-0.001416976892376853</v>
@@ -842,7 +842,7 @@
         <v>45237</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.004393994873672535</v>
+        <v>-0.02659778032912363</v>
       </c>
       <c r="C37" t="n">
         <v>0.006591440411184424</v>
@@ -853,7 +853,7 @@
         <v>45236</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.02721588819418908</v>
+        <v>-0.003341851779044558</v>
       </c>
       <c r="C38" t="n">
         <v>0.002767433987813206</v>
@@ -864,7 +864,7 @@
         <v>45233</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.009451795841209809</v>
+        <v>-0.01400394477317557</v>
       </c>
       <c r="C39" t="n">
         <v>0.02700494554683486</v>
@@ -875,7 +875,7 @@
         <v>45231</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.02671755725190839</v>
+        <v>0.005601120224044909</v>
       </c>
       <c r="C40" t="n">
         <v>0.0168723043201584</v>
@@ -886,7 +886,7 @@
         <v>45230</v>
       </c>
       <c r="B41" t="n">
-        <v>-0.01411764705882346</v>
+        <v>0.002387109608116056</v>
       </c>
       <c r="C41" t="n">
         <v>0.005438453062240001</v>
@@ -897,7 +897,7 @@
         <v>45229</v>
       </c>
       <c r="B42" t="n">
-        <v>0.009944311853619769</v>
+        <v>0.001587616590593255</v>
       </c>
       <c r="C42" t="n">
         <v>-0.006787230474576522</v>
@@ -908,7 +908,7 @@
         <v>45226</v>
       </c>
       <c r="B43" t="n">
-        <v>0.007877116975187004</v>
+        <v>0.005151575193184099</v>
       </c>
       <c r="C43" t="n">
         <v>-0.01285971928173768</v>
@@ -919,7 +919,7 @@
         <v>45225</v>
       </c>
       <c r="B44" t="n">
-        <v>0.01524032825322386</v>
+        <v>0.01517839542676924</v>
       </c>
       <c r="C44" t="n">
         <v>0.0172560489231588</v>
@@ -930,7 +930,7 @@
         <v>45224</v>
       </c>
       <c r="B45" t="n">
-        <v>-0.02424942263279439</v>
+        <v>-0.002135922330097073</v>
       </c>
       <c r="C45" t="n">
         <v>-0.008192542325205276</v>
@@ -941,7 +941,7 @@
         <v>45223</v>
       </c>
       <c r="B46" t="n">
-        <v>-0.001972386587771213</v>
+        <v>-0.001556723097878909</v>
       </c>
       <c r="C46" t="n">
         <v>0.008662499445848404</v>
@@ -952,7 +952,7 @@
         <v>45222</v>
       </c>
       <c r="B47" t="n">
-        <v>0</v>
+        <v>0.03586045605145194</v>
       </c>
       <c r="C47" t="n">
         <v>-0.00326985108921396</v>
@@ -963,7 +963,7 @@
         <v>45219</v>
       </c>
       <c r="B48" t="n">
-        <v>-0.0007905138339920903</v>
+        <v>0.009219190968955848</v>
       </c>
       <c r="C48" t="n">
         <v>-0.007447107119048502</v>
@@ -974,7 +974,7 @@
         <v>45218</v>
       </c>
       <c r="B49" t="n">
-        <v>0.003560126582278444</v>
+        <v>0.01976137211036555</v>
       </c>
       <c r="C49" t="n">
         <v>-0.0004909696650885476</v>
@@ -985,7 +985,7 @@
         <v>45217</v>
       </c>
       <c r="B50" t="n">
-        <v>-0.01143082380764693</v>
+        <v>0.001645338208409397</v>
       </c>
       <c r="C50" t="n">
         <v>-0.01594367946992448</v>
@@ -996,7 +996,7 @@
         <v>45216</v>
       </c>
       <c r="B51" t="n">
-        <v>0.02113237639553445</v>
+        <v>0.02482204781894515</v>
       </c>
       <c r="C51" t="n">
         <v>-0.005371822815658955</v>
@@ -1007,7 +1007,7 @@
         <v>45215</v>
       </c>
       <c r="B52" t="n">
-        <v>0.01522842639593902</v>
+        <v>-0.001602849510240367</v>
       </c>
       <c r="C52" t="n">
         <v>0.006738428045683031</v>
@@ -1018,7 +1018,7 @@
         <v>45212</v>
       </c>
       <c r="B53" t="n">
-        <v>-0.001538461538461489</v>
+        <v>0.02069211559043871</v>
       </c>
       <c r="C53" t="n">
         <v>-0.01108064006287857</v>
@@ -1029,7 +1029,7 @@
         <v>45210</v>
       </c>
       <c r="B54" t="n">
-        <v>0.01040061633281963</v>
+        <v>-0.03268088081090526</v>
       </c>
       <c r="C54" t="n">
         <v>0.002689807002064448</v>
@@ -1040,7 +1040,7 @@
         <v>45209</v>
       </c>
       <c r="B55" t="n">
-        <v>-0.01258101410598556</v>
+        <v>-0.003432700993676652</v>
       </c>
       <c r="C55" t="n">
         <v>0.01372920212581197</v>
@@ -1051,7 +1051,7 @@
         <v>45208</v>
       </c>
       <c r="B56" t="n">
-        <v>0.001158301158301178</v>
+        <v>0.00435097897026826</v>
       </c>
       <c r="C56" t="n">
         <v>0.008636244197249621</v>
@@ -1062,7 +1062,7 @@
         <v>45205</v>
       </c>
       <c r="B57" t="n">
-        <v>0.00887003470883152</v>
+        <v>-0.008844765342960303</v>
       </c>
       <c r="C57" t="n">
         <v>0.007821051516542443</v>
@@ -1073,7 +1073,7 @@
         <v>45204</v>
       </c>
       <c r="B58" t="n">
-        <v>-0.009556574923547445</v>
+        <v>-0.01675468949189574</v>
       </c>
       <c r="C58" t="n">
         <v>-0.002843134665997726</v>
@@ -1084,7 +1084,7 @@
         <v>45203</v>
       </c>
       <c r="B59" t="n">
-        <v>-0.01543805480509453</v>
+        <v>-0.004630487127245786</v>
       </c>
       <c r="C59" t="n">
         <v>0.001657570601045766</v>
@@ -1095,7 +1095,7 @@
         <v>45202</v>
       </c>
       <c r="B60" t="n">
-        <v>-0.02234417875343009</v>
+        <v>0.005024190547078478</v>
       </c>
       <c r="C60" t="n">
         <v>-0.01423642194738262</v>
@@ -1106,7 +1106,7 @@
         <v>45201</v>
       </c>
       <c r="B61" t="n">
-        <v>0.01283079390537289</v>
+        <v>-0.01907054249213114</v>
       </c>
       <c r="C61" t="n">
         <v>-0.01293698794663922</v>
@@ -1117,7 +1117,7 @@
         <v>45198</v>
       </c>
       <c r="B62" t="n">
-        <v>0.009105304829770233</v>
+        <v>0.001132502831257209</v>
       </c>
       <c r="C62" t="n">
         <v>0.007206366487803706</v>
@@ -1128,7 +1128,7 @@
         <v>45197</v>
       </c>
       <c r="B63" t="n">
-        <v>0.001569242840329554</v>
+        <v>-0.008295625942684737</v>
       </c>
       <c r="C63" t="n">
         <v>0.01228056364638275</v>
@@ -1139,7 +1139,7 @@
         <v>45196</v>
       </c>
       <c r="B64" t="n">
-        <v>-0.02585193889541715</v>
+        <v>0.004372623574144363</v>
       </c>
       <c r="C64" t="n">
         <v>0.00117345196290497</v>
@@ -1150,7 +1150,7 @@
         <v>45195</v>
       </c>
       <c r="B65" t="n">
-        <v>0.002010454362685987</v>
+        <v>0.005300018928638961</v>
       </c>
       <c r="C65" t="n">
         <v>-0.01494069441449208</v>
@@ -1161,10 +1161,2012 @@
         <v>45194</v>
       </c>
       <c r="B66" t="n">
-        <v>0.01484751203852319</v>
+        <v>0.015627942007155</v>
       </c>
       <c r="C66" t="n">
         <v>-0.0007240817522778942</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n">
+        <v>45191</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0.003151649981461002</v>
+      </c>
+      <c r="C67" t="n">
+        <v>-0.001170950105471635</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="n">
+        <v>45190</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0.0114581408242469</v>
+      </c>
+      <c r="C68" t="n">
+        <v>-0.02148363452546442</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45189</v>
+      </c>
+      <c r="B69" t="n">
+        <v>-0.02009866617942613</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.007204317499108992</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>45188</v>
+      </c>
+      <c r="B70" t="n">
+        <v>-0.0384113369382808</v>
+      </c>
+      <c r="C70" t="n">
+        <v>-0.003736642770188037</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>45187</v>
+      </c>
+      <c r="B71" t="n">
+        <v>-0.0137676943959667</v>
+      </c>
+      <c r="C71" t="n">
+        <v>-0.003957628117684742</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45184</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0.009241053873377814</v>
+      </c>
+      <c r="C72" t="n">
+        <v>-0.0053102385419459</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>45183</v>
+      </c>
+      <c r="B73" t="n">
+        <v>-0.02474186635495801</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.01028973734091521</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="n">
+        <v>45182</v>
+      </c>
+      <c r="B74" t="n">
+        <v>-0.0191769876148622</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.00176319001763181</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n">
+        <v>45181</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0.0004073319755599769</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.009282787060564734</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="n">
+        <v>45180</v>
+      </c>
+      <c r="B76" t="n">
+        <v>-0.006107491856677472</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.01361511711602326</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>45177</v>
+      </c>
+      <c r="B77" t="n">
+        <v>-0.02693877551020407</v>
+      </c>
+      <c r="C77" t="n">
+        <v>-0.005793852653360299</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="n">
+        <v>45175</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0.02181208053691264</v>
+      </c>
+      <c r="C78" t="n">
+        <v>-0.0114718190418559</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>45174</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0.01621510673234816</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-0.003786817460115333</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>45173</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.005857402544940493</v>
+      </c>
+      <c r="C80" t="n">
+        <v>-0.0009839430670184335</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B81" t="n">
+        <v>-0.02385141739980445</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.01858443780131669</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>45169</v>
+      </c>
+      <c r="B82" t="n">
+        <v>-0.0186260765071099</v>
+      </c>
+      <c r="C82" t="n">
+        <v>-0.01525503041647169</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>45168</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.01367346938775515</v>
+      </c>
+      <c r="C83" t="n">
+        <v>-0.007339279078409477</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>45167</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.006241191866317664</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.01095448297060297</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>45166</v>
+      </c>
+      <c r="B85" t="n">
+        <v>-0.0166066426570628</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.01108454120876745</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>45163</v>
+      </c>
+      <c r="B86" t="n">
+        <v>-0.007934893184130209</v>
+      </c>
+      <c r="C86" t="n">
+        <v>-0.01016013535453664</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>45162</v>
+      </c>
+      <c r="B87" t="n">
+        <v>-0.01107465135356844</v>
+      </c>
+      <c r="C87" t="n">
+        <v>-0.009387565073856186</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>45161</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.002695976773123165</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.01703743241847167</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>45160</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.007445708376421889</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.0150923279937778</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>45159</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0.004516526380619945</v>
+      </c>
+      <c r="C90" t="n">
+        <v>-0.008491538788136133</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="n">
+        <v>45156</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0.01205804210096062</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.00371362474126391</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="n">
+        <v>45155</v>
+      </c>
+      <c r="B92" t="n">
+        <v>-0.005452342487883732</v>
+      </c>
+      <c r="C92" t="n">
+        <v>-0.005277181811890075</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>45154</v>
+      </c>
+      <c r="B93" t="n">
+        <v>-0.009746192893400951</v>
+      </c>
+      <c r="C93" t="n">
+        <v>-0.00498403215948906</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="n">
+        <v>45153</v>
+      </c>
+      <c r="B94" t="n">
+        <v>0.002460529013737833</v>
+      </c>
+      <c r="C94" t="n">
+        <v>-0.005470422052906376</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>45152</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0.01759050930660666</v>
+      </c>
+      <c r="C95" t="n">
+        <v>-0.01062973785626564</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>45149</v>
+      </c>
+      <c r="B96" t="n">
+        <v>-0.01467336683417075</v>
+      </c>
+      <c r="C96" t="n">
+        <v>-0.002408111533586776</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>45148</v>
+      </c>
+      <c r="B97" t="n">
+        <v>-0.01631986944104458</v>
+      </c>
+      <c r="C97" t="n">
+        <v>-0.0004982729353343318</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>45147</v>
+      </c>
+      <c r="B98" t="n">
+        <v>-0.001036914143508816</v>
+      </c>
+      <c r="C98" t="n">
+        <v>-0.005718364262322639</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>45146</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0.009134315964293149</v>
+      </c>
+      <c r="C99" t="n">
+        <v>-0.002429217624392743</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>45145</v>
+      </c>
+      <c r="B100" t="n">
+        <v>0.01542892408969343</v>
+      </c>
+      <c r="C100" t="n">
+        <v>-0.001071058004485037</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>45142</v>
+      </c>
+      <c r="B101" t="n">
+        <v>-0.004862236628849326</v>
+      </c>
+      <c r="C101" t="n">
+        <v>-0.00893967790622463</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="n">
+        <v>45141</v>
+      </c>
+      <c r="B102" t="n">
+        <v>-0.0126221498371335</v>
+      </c>
+      <c r="C102" t="n">
+        <v>-0.002258830538064971</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>45140</v>
+      </c>
+      <c r="B103" t="n">
+        <v>-0.03525773195876292</v>
+      </c>
+      <c r="C103" t="n">
+        <v>-0.003208300343098491</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B104" t="n">
+        <v>0.0102586022654414</v>
+      </c>
+      <c r="C104" t="n">
+        <v>-0.005699384138490915</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>45138</v>
+      </c>
+      <c r="B105" t="n">
+        <v>-0.006346519991538013</v>
+      </c>
+      <c r="C105" t="n">
+        <v>0.01461056520255943</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>45135</v>
+      </c>
+      <c r="B106" t="n">
+        <v>-0.0178837555886735</v>
+      </c>
+      <c r="C106" t="n">
+        <v>0.001641803483623638</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>45134</v>
+      </c>
+      <c r="B107" t="n">
+        <v>-0.0002167786689790674</v>
+      </c>
+      <c r="C107" t="n">
+        <v>-0.0209693211488251</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>45133</v>
+      </c>
+      <c r="B108" t="n">
+        <v>-0.01539462272333048</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0.004524293488951558</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="n">
+        <v>45132</v>
+      </c>
+      <c r="B109" t="n">
+        <v>-0.02686632900242236</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0.005488618944800683</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="n">
+        <v>45131</v>
+      </c>
+      <c r="B110" t="n">
+        <v>-0.004525910839556335</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0.009358077476563142</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="n">
+        <v>45128</v>
+      </c>
+      <c r="B111" t="n">
+        <v>-0.02136849283928177</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0.01807203407772495</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="n">
+        <v>45127</v>
+      </c>
+      <c r="B112" t="n">
+        <v>-0.009291521486643362</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0.004517149857084624</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>45126</v>
+      </c>
+      <c r="B113" t="n">
+        <v>-0.004220398593200447</v>
+      </c>
+      <c r="C113" t="n">
+        <v>-0.002452457124430429</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>45125</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0.02542971509300673</v>
+      </c>
+      <c r="C114" t="n">
+        <v>-0.003197455569747709</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>45124</v>
+      </c>
+      <c r="B115" t="n">
+        <v>-0.00390355912743956</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0.004315654441810812</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>45121</v>
+      </c>
+      <c r="B116" t="n">
+        <v>0.003457814661134151</v>
+      </c>
+      <c r="C116" t="n">
+        <v>-0.01302153206332168</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>45120</v>
+      </c>
+      <c r="B117" t="n">
+        <v>-0.004135079255685681</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0.01358081348902829</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>45119</v>
+      </c>
+      <c r="B118" t="n">
+        <v>-0.004152249134948049</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0.003804811465620173</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>45118</v>
+      </c>
+      <c r="B119" t="n">
+        <v>-0.003011350474866892</v>
+      </c>
+      <c r="C119" t="n">
+        <v>-0.006121653015889184</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>45117</v>
+      </c>
+      <c r="B120" t="n">
+        <v>-0.0004646840148697651</v>
+      </c>
+      <c r="C120" t="n">
+        <v>-0.008040505307069901</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="n">
+        <v>45114</v>
+      </c>
+      <c r="B121" t="n">
+        <v>0.01092515109251502</v>
+      </c>
+      <c r="C121" t="n">
+        <v>0.01253555430654196</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>45113</v>
+      </c>
+      <c r="B122" t="n">
+        <v>-0.008967578753736549</v>
+      </c>
+      <c r="C122" t="n">
+        <v>-0.01775840868597811</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>45112</v>
+      </c>
+      <c r="B123" t="n">
+        <v>0.007656612529002293</v>
+      </c>
+      <c r="C123" t="n">
+        <v>0.003972253014881355</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>45111</v>
+      </c>
+      <c r="B124" t="n">
+        <v>0.006447156343541316</v>
+      </c>
+      <c r="C124" t="n">
+        <v>-0.004988593918427764</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>45110</v>
+      </c>
+      <c r="B125" t="n">
+        <v>-0.01143902997025847</v>
+      </c>
+      <c r="C125" t="n">
+        <v>0.01343077561458927</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="n">
+        <v>45107</v>
+      </c>
+      <c r="B126" t="n">
+        <v>0</v>
+      </c>
+      <c r="C126" t="n">
+        <v>-0.002500359004248942</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="n">
+        <v>45106</v>
+      </c>
+      <c r="B127" t="n">
+        <v>-0.003934274473501587</v>
+      </c>
+      <c r="C127" t="n">
+        <v>0.01458677933853836</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="n">
+        <v>45105</v>
+      </c>
+      <c r="B128" t="n">
+        <v>0.002788104089219257</v>
+      </c>
+      <c r="C128" t="n">
+        <v>-0.007164555023272068</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="n">
+        <v>45104</v>
+      </c>
+      <c r="B129" t="n">
+        <v>0.01506024096385561</v>
+      </c>
+      <c r="C129" t="n">
+        <v>-0.006089155383405376</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>45103</v>
+      </c>
+      <c r="B130" t="n">
+        <v>0.01711937913718331</v>
+      </c>
+      <c r="C130" t="n">
+        <v>-0.006169259604797528</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="n">
+        <v>45100</v>
+      </c>
+      <c r="B131" t="n">
+        <v>0.007405745062836644</v>
+      </c>
+      <c r="C131" t="n">
+        <v>0.0003615450586038627</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="n">
+        <v>45099</v>
+      </c>
+      <c r="B132" t="n">
+        <v>-0.00178213410559136</v>
+      </c>
+      <c r="C132" t="n">
+        <v>-0.01234014283341633</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="2" t="n">
+        <v>45098</v>
+      </c>
+      <c r="B133" t="n">
+        <v>0.01338986833296119</v>
+      </c>
+      <c r="C133" t="n">
+        <v>0.006671013693133387</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45097</v>
+      </c>
+      <c r="B134" t="n">
+        <v>0.02070028628055498</v>
+      </c>
+      <c r="C134" t="n">
+        <v>-0.001968996646031118</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>45096</v>
+      </c>
+      <c r="B135" t="n">
+        <v>0.005609492988133624</v>
+      </c>
+      <c r="C135" t="n">
+        <v>0.009262533892453462</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45093</v>
+      </c>
+      <c r="B136" t="n">
+        <v>0.01244368161338771</v>
+      </c>
+      <c r="C136" t="n">
+        <v>-0.003883544006508921</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B137" t="n">
+        <v>0.0008476372112735664</v>
+      </c>
+      <c r="C137" t="n">
+        <v>0.001276570727897219</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>45091</v>
+      </c>
+      <c r="B138" t="n">
+        <v>-0.03493542240101633</v>
+      </c>
+      <c r="C138" t="n">
+        <v>0.01992410679869461</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>45090</v>
+      </c>
+      <c r="B139" t="n">
+        <v>0.008556384379113657</v>
+      </c>
+      <c r="C139" t="n">
+        <v>-0.005053862412217947</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="2" t="n">
+        <v>45089</v>
+      </c>
+      <c r="B140" t="n">
+        <v>-0.007396127909506167</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0.00270896179252933</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>45086</v>
+      </c>
+      <c r="B141" t="n">
+        <v>-0.03133903133903138</v>
+      </c>
+      <c r="C141" t="n">
+        <v>0.01325678858409529</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>45084</v>
+      </c>
+      <c r="B142" t="n">
+        <v>0.01312217194570131</v>
+      </c>
+      <c r="C142" t="n">
+        <v>0.007660762586161773</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="n">
+        <v>45083</v>
+      </c>
+      <c r="B143" t="n">
+        <v>0.02411790978115236</v>
+      </c>
+      <c r="C143" t="n">
+        <v>0.0169837438773337</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="n">
+        <v>45082</v>
+      </c>
+      <c r="B144" t="n">
+        <v>-0.002616659398168242</v>
+      </c>
+      <c r="C144" t="n">
+        <v>0.001226034577728852</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="n">
+        <v>45079</v>
+      </c>
+      <c r="B145" t="n">
+        <v>-0.008307826847398392</v>
+      </c>
+      <c r="C145" t="n">
+        <v>0.01802559580337348</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B146" t="n">
+        <v>-0.03064373897707229</v>
+      </c>
+      <c r="C146" t="n">
+        <v>0.02058429870309686</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="n">
+        <v>45077</v>
+      </c>
+      <c r="B147" t="n">
+        <v>-0.005003411416875103</v>
+      </c>
+      <c r="C147" t="n">
+        <v>-0.005799921077023318</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>45076</v>
+      </c>
+      <c r="B148" t="n">
+        <v>0.00777142857142854</v>
+      </c>
+      <c r="C148" t="n">
+        <v>-0.01238070205650166</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45075</v>
+      </c>
+      <c r="B149" t="n">
+        <v>0.005670220004536208</v>
+      </c>
+      <c r="C149" t="n">
+        <v>-0.005166537428092255</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>45072</v>
+      </c>
+      <c r="B150" t="n">
+        <v>-0.0006765899864682456</v>
+      </c>
+      <c r="C150" t="n">
+        <v>0.007741654097079609</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="2" t="n">
+        <v>45071</v>
+      </c>
+      <c r="B151" t="n">
+        <v>-0.02708192281652</v>
+      </c>
+      <c r="C151" t="n">
+        <v>0.0115257352941176</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>45070</v>
+      </c>
+      <c r="B152" t="n">
+        <v>0.01067037810252836</v>
+      </c>
+      <c r="C152" t="n">
+        <v>-0.0102702653530915</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>45069</v>
+      </c>
+      <c r="B153" t="n">
+        <v>0.02845994950654118</v>
+      </c>
+      <c r="C153" t="n">
+        <v>-0.00257682850480434</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="n">
+        <v>45068</v>
+      </c>
+      <c r="B154" t="n">
+        <v>-0.01495201963847359</v>
+      </c>
+      <c r="C154" t="n">
+        <v>-0.004803828615287387</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="2" t="n">
+        <v>45065</v>
+      </c>
+      <c r="B155" t="n">
+        <v>0.005437245129134682</v>
+      </c>
+      <c r="C155" t="n">
+        <v>0.005785229047843954</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B156" t="n">
+        <v>-0.001577287066246047</v>
+      </c>
+      <c r="C156" t="n">
+        <v>0.005919970765576377</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="2" t="n">
+        <v>45063</v>
+      </c>
+      <c r="B157" t="n">
+        <v>-0.03565786504175139</v>
+      </c>
+      <c r="C157" t="n">
+        <v>0.01170120339390346</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45062</v>
+      </c>
+      <c r="B158" t="n">
+        <v>-0.0004680552305170727</v>
+      </c>
+      <c r="C158" t="n">
+        <v>-0.007658512872721901</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="n">
+        <v>45061</v>
+      </c>
+      <c r="B159" t="n">
+        <v>-0.01826270194333879</v>
+      </c>
+      <c r="C159" t="n">
+        <v>0.005209101637409619</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="2" t="n">
+        <v>45058</v>
+      </c>
+      <c r="B160" t="n">
+        <v>-0.01097066539470548</v>
+      </c>
+      <c r="C160" t="n">
+        <v>0.001921371563700758</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>45057</v>
+      </c>
+      <c r="B161" t="n">
+        <v>-0.02049674463467566</v>
+      </c>
+      <c r="C161" t="n">
+        <v>0.007519916610825739</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="n">
+        <v>45056</v>
+      </c>
+      <c r="B162" t="n">
+        <v>0.002708025603151087</v>
+      </c>
+      <c r="C162" t="n">
+        <v>0.003118173161304805</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="n">
+        <v>45055</v>
+      </c>
+      <c r="B163" t="n">
+        <v>-0.004419346918733136</v>
+      </c>
+      <c r="C163" t="n">
+        <v>0.01010920201429633</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>45054</v>
+      </c>
+      <c r="B164" t="n">
+        <v>0.008877928483353781</v>
+      </c>
+      <c r="C164" t="n">
+        <v>0.008502301517860467</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="2" t="n">
+        <v>45051</v>
+      </c>
+      <c r="B165" t="n">
+        <v>-0.02587446094873036</v>
+      </c>
+      <c r="C165" t="n">
+        <v>0.02910720927046029</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>45050</v>
+      </c>
+      <c r="B166" t="n">
+        <v>-0.04845056566650263</v>
+      </c>
+      <c r="C166" t="n">
+        <v>0.003703449021090988</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45049</v>
+      </c>
+      <c r="B167" t="n">
+        <v>0.01266477125872334</v>
+      </c>
+      <c r="C167" t="n">
+        <v>-0.001275422606375143</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="n">
+        <v>45048</v>
+      </c>
+      <c r="B168" t="n">
+        <v>0.01454823889739654</v>
+      </c>
+      <c r="C168" t="n">
+        <v>-0.02398690056687602</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="n">
+        <v>45044</v>
+      </c>
+      <c r="B169" t="n">
+        <v>-0.02163522012578611</v>
+      </c>
+      <c r="C169" t="n">
+        <v>0.01466144593531093</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="n">
+        <v>45043</v>
+      </c>
+      <c r="B170" t="n">
+        <v>-0.04525584983286191</v>
+      </c>
+      <c r="C170" t="n">
+        <v>0.005971929001485687</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="2" t="n">
+        <v>45042</v>
+      </c>
+      <c r="B171" t="n">
+        <v>0.00673309991920279</v>
+      </c>
+      <c r="C171" t="n">
+        <v>-0.008796744816895963</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="n">
+        <v>45041</v>
+      </c>
+      <c r="B172" t="n">
+        <v>0.01417870518994091</v>
+      </c>
+      <c r="C172" t="n">
+        <v>-0.006993948839312369</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="2" t="n">
+        <v>45040</v>
+      </c>
+      <c r="B173" t="n">
+        <v>0.02242152466367719</v>
+      </c>
+      <c r="C173" t="n">
+        <v>-0.004024260542125346</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="n">
+        <v>45036</v>
+      </c>
+      <c r="B174" t="n">
+        <v>0.01599587203302377</v>
+      </c>
+      <c r="C174" t="n">
+        <v>0.004369039484953818</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="n">
+        <v>45035</v>
+      </c>
+      <c r="B175" t="n">
+        <v>0.02209243270695782</v>
+      </c>
+      <c r="C175" t="n">
+        <v>-0.02119382459048824</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B176" t="n">
+        <v>-0.0004968944099379424</v>
+      </c>
+      <c r="C176" t="n">
+        <v>0.001386583157259258</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="2" t="n">
+        <v>45033</v>
+      </c>
+      <c r="B177" t="n">
+        <v>-0.01739995028585617</v>
+      </c>
+      <c r="C177" t="n">
+        <v>-0.002474618692309916</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2" t="n">
+        <v>45030</v>
+      </c>
+      <c r="B178" t="n">
+        <v>0.0007589172780166908</v>
+      </c>
+      <c r="C178" t="n">
+        <v>-0.001681414266659131</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="n">
+        <v>45029</v>
+      </c>
+      <c r="B179" t="n">
+        <v>0.02022244691607678</v>
+      </c>
+      <c r="C179" t="n">
+        <v>-0.004041538029750158</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="n">
+        <v>45028</v>
+      </c>
+      <c r="B180" t="n">
+        <v>0.02155599603567881</v>
+      </c>
+      <c r="C180" t="n">
+        <v>0.00636450938670996</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="n">
+        <v>45027</v>
+      </c>
+      <c r="B181" t="n">
+        <v>0.008246422507882656</v>
+      </c>
+      <c r="C181" t="n">
+        <v>0.04287804255402716</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="n">
+        <v>45026</v>
+      </c>
+      <c r="B182" t="n">
+        <v>-0.03295645898484478</v>
+      </c>
+      <c r="C182" t="n">
+        <v>0.01016643192953914</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="2" t="n">
+        <v>45022</v>
+      </c>
+      <c r="B183" t="n">
+        <v>-0.01890547263681608</v>
+      </c>
+      <c r="C183" t="n">
+        <v>-0.001544890966349133</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="2" t="n">
+        <v>45021</v>
+      </c>
+      <c r="B184" t="n">
+        <v>0.01521298174442198</v>
+      </c>
+      <c r="C184" t="n">
+        <v>-0.008746527402840876</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="2" t="n">
+        <v>45020</v>
+      </c>
+      <c r="B185" t="n">
+        <v>0.03346653346653361</v>
+      </c>
+      <c r="C185" t="n">
+        <v>0.003576143282170596</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="2" t="n">
+        <v>45019</v>
+      </c>
+      <c r="B186" t="n">
+        <v>0.009183180280328607</v>
+      </c>
+      <c r="C186" t="n">
+        <v>-0.003690543962623472</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="2" t="n">
+        <v>45016</v>
+      </c>
+      <c r="B187" t="n">
+        <v>-0.02658045977011492</v>
+      </c>
+      <c r="C187" t="n">
+        <v>-0.01765448882975129</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="2" t="n">
+        <v>45015</v>
+      </c>
+      <c r="B188" t="n">
+        <v>0.03468634686346883</v>
+      </c>
+      <c r="C188" t="n">
+        <v>0.01886180778639002</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="2" t="n">
+        <v>45014</v>
+      </c>
+      <c r="B189" t="n">
+        <v>0.0004755111745124996</v>
+      </c>
+      <c r="C189" t="n">
+        <v>0.006008795770124031</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="2" t="n">
+        <v>45013</v>
+      </c>
+      <c r="B190" t="n">
+        <v>-0.01829847908745241</v>
+      </c>
+      <c r="C190" t="n">
+        <v>0.01520016052974826</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="2" t="n">
+        <v>45012</v>
+      </c>
+      <c r="B191" t="n">
+        <v>-0.006778019849915329</v>
+      </c>
+      <c r="C191" t="n">
+        <v>0.008509647977820167</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="2" t="n">
+        <v>45009</v>
+      </c>
+      <c r="B192" t="n">
+        <v>0.01511089446746272</v>
+      </c>
+      <c r="C192" t="n">
+        <v>0.009221248697996343</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="2" t="n">
+        <v>45008</v>
+      </c>
+      <c r="B193" t="n">
+        <v>-0.009123649459783834</v>
+      </c>
+      <c r="C193" t="n">
+        <v>-0.02289939234292215</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="2" t="n">
+        <v>45007</v>
+      </c>
+      <c r="B194" t="n">
+        <v>0.01526532590259255</v>
+      </c>
+      <c r="C194" t="n">
+        <v>-0.007693221647953385</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="2" t="n">
+        <v>45006</v>
+      </c>
+      <c r="B195" t="n">
+        <v>0.001670644391408072</v>
+      </c>
+      <c r="C195" t="n">
+        <v>0.0007431408103206749</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="2" t="n">
+        <v>45005</v>
+      </c>
+      <c r="B196" t="n">
+        <v>0.006433166547534119</v>
+      </c>
+      <c r="C196" t="n">
+        <v>-0.01038418544449016</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="2" t="n">
+        <v>45002</v>
+      </c>
+      <c r="B197" t="n">
+        <v>0.008285984848484862</v>
+      </c>
+      <c r="C197" t="n">
+        <v>-0.01404746942524293</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="2" t="n">
+        <v>45001</v>
+      </c>
+      <c r="B198" t="n">
+        <v>0.00915707912655539</v>
+      </c>
+      <c r="C198" t="n">
+        <v>0.007401996591185789</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="2" t="n">
+        <v>45000</v>
+      </c>
+      <c r="B199" t="n">
+        <v>0.005351326198231865</v>
+      </c>
+      <c r="C199" t="n">
+        <v>-0.002496793999922309</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="2" t="n">
+        <v>44999</v>
+      </c>
+      <c r="B200" t="n">
+        <v>0.01689423744503582</v>
+      </c>
+      <c r="C200" t="n">
+        <v>-0.001832798363088028</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="2" t="n">
+        <v>44998</v>
+      </c>
+      <c r="B201" t="n">
+        <v>-0.008648156577150568</v>
+      </c>
+      <c r="C201" t="n">
+        <v>-0.004796463934837569</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="2" t="n">
+        <v>44995</v>
+      </c>
+      <c r="B202" t="n">
+        <v>0.01101928374655636</v>
+      </c>
+      <c r="C202" t="n">
+        <v>-0.01382874437285264</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="2" t="n">
+        <v>44994</v>
+      </c>
+      <c r="B203" t="n">
+        <v>0.03110808356039962</v>
+      </c>
+      <c r="C203" t="n">
+        <v>-0.01378824854514737</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="2" t="n">
+        <v>44993</v>
+      </c>
+      <c r="B204" t="n">
+        <v>0.02070028628055498</v>
+      </c>
+      <c r="C204" t="n">
+        <v>0.02218213915646472</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="2" t="n">
+        <v>44992</v>
+      </c>
+      <c r="B205" t="n">
+        <v>0.006688241639697834</v>
+      </c>
+      <c r="C205" t="n">
+        <v>-0.004508118433619868</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="2" t="n">
+        <v>44991</v>
+      </c>
+      <c r="B206" t="n">
+        <v>0.0006429489927133325</v>
+      </c>
+      <c r="C206" t="n">
+        <v>0.00802957656981107</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="2" t="n">
+        <v>44988</v>
+      </c>
+      <c r="B207" t="n">
+        <v>0.008781323623902493</v>
+      </c>
+      <c r="C207" t="n">
+        <v>0.005226177341617788</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="2" t="n">
+        <v>44987</v>
+      </c>
+      <c r="B208" t="n">
+        <v>-0.03121019108280254</v>
+      </c>
+      <c r="C208" t="n">
+        <v>-0.01014513579537291</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="2" t="n">
+        <v>44986</v>
+      </c>
+      <c r="B209" t="n">
+        <v>0.001534078457155363</v>
+      </c>
+      <c r="C209" t="n">
+        <v>-0.00521289978271644</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="2" t="n">
+        <v>44985</v>
+      </c>
+      <c r="B210" t="n">
+        <v>0.02078774617067825</v>
+      </c>
+      <c r="C210" t="n">
+        <v>-0.007369147960004208</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="B211" t="n">
+        <v>-0.02936763129689168</v>
+      </c>
+      <c r="C211" t="n">
+        <v>-0.001530135161939339</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="2" t="n">
+        <v>44981</v>
+      </c>
+      <c r="B212" t="n">
+        <v>-0.004196113074204866</v>
+      </c>
+      <c r="C212" t="n">
+        <v>-0.01714630523579652</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="2" t="n">
+        <v>44980</v>
+      </c>
+      <c r="B213" t="n">
+        <v>0</v>
+      </c>
+      <c r="C213" t="n">
+        <v>0.005300880991488732</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="2" t="n">
+        <v>44979</v>
+      </c>
+      <c r="B214" t="n">
+        <v>-0.002439565313816949</v>
+      </c>
+      <c r="C214" t="n">
+        <v>-0.01967924027702805</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="2" t="n">
+        <v>44974</v>
+      </c>
+      <c r="B215" t="n">
+        <v>0.02000889284126295</v>
+      </c>
+      <c r="C215" t="n">
+        <v>-0.005477457804467512</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="2" t="n">
+        <v>44973</v>
+      </c>
+      <c r="B216" t="n">
+        <v>0.01721883173496064</v>
+      </c>
+      <c r="C216" t="n">
+        <v>0.004230551342263578</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="2" t="n">
+        <v>44972</v>
+      </c>
+      <c r="B217" t="n">
+        <v>0.008785086779515616</v>
+      </c>
+      <c r="C217" t="n">
+        <v>0.01656155082250432</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="2" t="n">
+        <v>44971</v>
+      </c>
+      <c r="B218" t="n">
+        <v>-0.02570093457943923</v>
+      </c>
+      <c r="C218" t="n">
+        <v>-0.01090531576723075</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="2" t="n">
+        <v>44970</v>
+      </c>
+      <c r="B219" t="n">
+        <v>-0.00501417048179631</v>
+      </c>
+      <c r="C219" t="n">
+        <v>0.00643550624133149</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="2" t="n">
+        <v>44967</v>
+      </c>
+      <c r="B220" t="n">
+        <v>-0.006573181419807117</v>
+      </c>
+      <c r="C220" t="n">
+        <v>0.003404989655140467</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="2" t="n">
+        <v>44966</v>
+      </c>
+      <c r="B221" t="n">
+        <v>-0.002205558006175612</v>
+      </c>
+      <c r="C221" t="n">
+        <v>-0.01910230975045957</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="2" t="n">
+        <v>44965</v>
+      </c>
+      <c r="B222" t="n">
+        <v>-0.007515473032714493</v>
+      </c>
+      <c r="C222" t="n">
+        <v>0.01818013343217206</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="2" t="n">
+        <v>44964</v>
+      </c>
+      <c r="B223" t="n">
+        <v>0.00222717149220486</v>
+      </c>
+      <c r="C223" t="n">
+        <v>-0.004942096333997226</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="2" t="n">
+        <v>44963</v>
+      </c>
+      <c r="B224" t="n">
+        <v>-0.002000000000000113</v>
+      </c>
+      <c r="C224" t="n">
+        <v>-0.000313392939441437</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="2" t="n">
+        <v>44960</v>
+      </c>
+      <c r="B225" t="n">
+        <v>0.007570696949454447</v>
+      </c>
+      <c r="C225" t="n">
+        <v>-0.01314413062264064</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="2" t="n">
+        <v>44959</v>
+      </c>
+      <c r="B226" t="n">
+        <v>-0.02784530386740325</v>
+      </c>
+      <c r="C226" t="n">
+        <v>-0.02108581248942598</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="2" t="n">
+        <v>44958</v>
+      </c>
+      <c r="B227" t="n">
+        <v>0.03841782223232548</v>
+      </c>
+      <c r="C227" t="n">
+        <v>-0.01082514181023853</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="2" t="n">
+        <v>44957</v>
+      </c>
+      <c r="B228" t="n">
+        <v>-0.008318739054290814</v>
+      </c>
+      <c r="C228" t="n">
+        <v>0.01469326469326471</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="2" t="n">
+        <v>44956</v>
+      </c>
+      <c r="B229" t="n">
+        <v>-0.001766004415010958</v>
+      </c>
+      <c r="C229" t="n">
+        <v>-0.005457680752342209</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="2" t="n">
+        <v>44953</v>
+      </c>
+      <c r="B230" t="n">
+        <v>-0.02587350729765592</v>
+      </c>
+      <c r="C230" t="n">
+        <v>-0.01408302587876509</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="2" t="n">
+        <v>44952</v>
+      </c>
+      <c r="B231" t="n">
+        <v>0.007037457434733385</v>
+      </c>
+      <c r="C231" t="n">
+        <v>-0.000753097771356015</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="2" t="n">
+        <v>44951</v>
+      </c>
+      <c r="B232" t="n">
+        <v>0.03020739404869266</v>
+      </c>
+      <c r="C232" t="n">
+        <v>0.01032487525214987</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="2" t="n">
+        <v>44950</v>
+      </c>
+      <c r="B233" t="n">
+        <v>0.01575492341356677</v>
+      </c>
+      <c r="C233" t="n">
+        <v>0.01180746403602217</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="2" t="n">
+        <v>44949</v>
+      </c>
+      <c r="B234" t="n">
+        <v>-0.01120206807410606</v>
+      </c>
+      <c r="C234" t="n">
+        <v>-0.005271547003143362</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="2" t="n">
+        <v>44946</v>
+      </c>
+      <c r="B235" t="n">
+        <v>0.003485838779956563</v>
+      </c>
+      <c r="C235" t="n">
+        <v>-0.006238606799638946</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="2" t="n">
+        <v>44945</v>
+      </c>
+      <c r="B236" t="n">
+        <v>0.04667824576639168</v>
+      </c>
+      <c r="C236" t="n">
+        <v>0.004926546437591162</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="2" t="n">
+        <v>44944</v>
+      </c>
+      <c r="B237" t="n">
+        <v>0.01057871810827615</v>
+      </c>
+      <c r="C237" t="n">
+        <v>0.009090174893888081</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="2" t="n">
+        <v>44943</v>
+      </c>
+      <c r="B238" t="n">
+        <v>0.02729885057471271</v>
+      </c>
+      <c r="C238" t="n">
+        <v>0.02038218893355181</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="2" t="n">
+        <v>44942</v>
+      </c>
+      <c r="B239" t="n">
+        <v>-0.01198801198801192</v>
+      </c>
+      <c r="C239" t="n">
+        <v>-0.01535396155649316</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="2" t="n">
+        <v>44939</v>
+      </c>
+      <c r="B240" t="n">
+        <v>-0.003640040444893855</v>
+      </c>
+      <c r="C240" t="n">
+        <v>-0.008589790573576339</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="2" t="n">
+        <v>44938</v>
+      </c>
+      <c r="B241" t="n">
+        <v>-0.003247412218388535</v>
+      </c>
+      <c r="C241" t="n">
+        <v>0.001020015568658605</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="2" t="n">
+        <v>44937</v>
+      </c>
+      <c r="B242" t="n">
+        <v>-0.02015882712278561</v>
+      </c>
+      <c r="C242" t="n">
+        <v>0.007672749567224413</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="2" t="n">
+        <v>44936</v>
+      </c>
+      <c r="B243" t="n">
+        <v>0.01475477971737327</v>
+      </c>
+      <c r="C243" t="n">
+        <v>0.01542658866397506</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="2" t="n">
+        <v>44935</v>
+      </c>
+      <c r="B244" t="n">
+        <v>0.01269711243088278</v>
+      </c>
+      <c r="C244" t="n">
+        <v>0.003592561284869067</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="2" t="n">
+        <v>44932</v>
+      </c>
+      <c r="B245" t="n">
+        <v>-0.01314459049545003</v>
+      </c>
+      <c r="C245" t="n">
+        <v>0.01225841254487614</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="2" t="n">
+        <v>44931</v>
+      </c>
+      <c r="B246" t="n">
+        <v>0.006352459016393475</v>
+      </c>
+      <c r="C246" t="n">
+        <v>0.02073404598705064</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="2" t="n">
+        <v>44930</v>
+      </c>
+      <c r="B247" t="n">
+        <v>-0.00610873549175317</v>
+      </c>
+      <c r="C247" t="n">
+        <v>0.01121287176237917</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="2" t="n">
+        <v>44929</v>
+      </c>
+      <c r="B248" t="n">
+        <v>-0.002048760499897551</v>
+      </c>
+      <c r="C248" t="n">
+        <v>-0.02077536286380388</v>
       </c>
     </row>
   </sheetData>
@@ -1198,7 +3200,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.008213876453595021</v>
+        <v>-0.1794044374275717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cria funções para exportar gráficos diretamente no excel, inclui mudanças nas funções principais e testa funcionalidade de gráficos
</commit_message>
<xml_diff>
--- a/doc/resultados_beta.xlsx
+++ b/doc/resultados_beta.xlsx
@@ -1,41 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Retornos" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Beta" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Retornos" sheetId="1" r:id="rId1"/>
+    <sheet name="Beta" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>acao</t>
+  </si>
+  <si>
+    <t>mercado</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -50,96 +67,38 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -427,2783 +386,2771 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C248"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="25.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>acao</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>mercado</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2">
         <v>45288</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>0.00888647080159588</v>
       </c>
-      <c r="C2" t="n">
-        <v>-6.706708198578326e-05</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="C2">
+        <v>-6.706708198578326E-05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2">
         <v>45287</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>-0.001438072982203997</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>0.004950087244351531</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
+    <row r="4" spans="1:3">
+      <c r="A4" s="2">
         <v>45286</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>-0.005940594059405946</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>0.005875573433368642</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
         <v>45282</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>-0.005070626584570803</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>0.00431980148583011</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
+    <row r="6" spans="1:3">
+      <c r="A6" s="2">
         <v>45281</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>-0.008918820531488847</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>0.01053484602917343</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
+    <row r="7" spans="1:3">
+      <c r="A7" s="2">
         <v>45280</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>-0.01010101010101017</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>-0.007940781639881433</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
+    <row r="8" spans="1:3">
+      <c r="A8" s="2">
         <v>45279</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>-0.01725417439703159</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>0.005851209911202027</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
+    <row r="9" spans="1:3">
+      <c r="A9" s="2">
         <v>45278</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>-0.007929016424391144</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>0.006812752982019665</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
+    <row r="10" spans="1:3">
+      <c r="A10" s="2">
         <v>45275</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>0.001522359657469163</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>-0.004929609758334452</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
+    <row r="11" spans="1:3">
+      <c r="A11" s="2">
         <v>45274</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>-0.004180125403762225</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>0.01063607924921794</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
+    <row r="12" spans="1:3">
+      <c r="A12" s="2">
         <v>45273</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>-0.010684983781721</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>0.02422410860501722</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
+    <row r="13" spans="1:3">
+      <c r="A13" s="2">
         <v>45272</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>-0.01716489874638383</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>-0.004042043556367947</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="n">
+    <row r="14" spans="1:3">
+      <c r="A14" s="2">
         <v>45271</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>0.008634222919937207</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>-0.001400538184336053</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
+    <row r="15" spans="1:3">
+      <c r="A15" s="2">
         <v>45268</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>-0.01225680933852136</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>0.008602491865725037</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
+    <row r="16" spans="1:3">
+      <c r="A16" s="2">
         <v>45267</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>-0.02028757140043336</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>0.003080646060036774</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="2" t="n">
+    <row r="17" spans="1:3">
+      <c r="A17" s="2">
         <v>45266</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>0.003216726980297402</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>-0.01008644397689573</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="2" t="n">
+    <row r="18" spans="1:3">
+      <c r="A18" s="2">
         <v>45265</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>0.007414829659318833</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>0.0007886248748059099</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="2" t="n">
+    <row r="19" spans="1:3">
+      <c r="A19" s="2">
         <v>45264</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>0.006564551422319376</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19">
         <v>-0.01014808396368549</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="2" t="n">
+    <row r="20" spans="1:3">
+      <c r="A20" s="2">
         <v>45261</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>-0.0005928853754940677</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20">
         <v>0.006062938326095058</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="2" t="n">
+    <row r="21" spans="1:3">
+      <c r="A21" s="2">
         <v>45260</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>0.03915364840814717</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>0.00975408601042016</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="2" t="n">
+    <row r="22" spans="1:3">
+      <c r="A22" s="2">
         <v>45259</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>0.008753568030447134</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>-0.003453508037111419</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="2" t="n">
+    <row r="23" spans="1:3">
+      <c r="A23" s="2">
         <v>45258</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>-0.01660064138841721</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23">
         <v>0.006802829340483596</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="2" t="n">
+    <row r="24" spans="1:3">
+      <c r="A24" s="2">
         <v>45257</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>0.007481296758104827</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24">
         <v>0.001123130107852255</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="2" t="n">
+    <row r="25" spans="1:3">
+      <c r="A25" s="2">
         <v>45254</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>-0.005331302361005319</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25">
         <v>-0.008169005182657063</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="2" t="n">
+    <row r="26" spans="1:3">
+      <c r="A26" s="2">
         <v>45253</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>0.00631699846860645</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26">
         <v>0.004292458444083103</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="2" t="n">
+    <row r="27" spans="1:3">
+      <c r="A27" s="2">
         <v>45252</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>-0.0068480121742438</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27">
         <v>0.003407453406259142</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="2" t="n">
+    <row r="28" spans="1:3">
+      <c r="A28" s="2">
         <v>45251</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>-0.008427504309519218</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28">
         <v>-0.003870097942027861</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="2" t="n">
+    <row r="29" spans="1:3">
+      <c r="A29" s="2">
         <v>45250</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>-0.00154529650376678</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29">
         <v>0.008259903088068343</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="2" t="n">
+    <row r="30" spans="1:3">
+      <c r="A30" s="2">
         <v>45247</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>0.0007738440704196936</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30">
         <v>0.003901232982275848</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="2" t="n">
+    <row r="31" spans="1:3">
+      <c r="A31" s="2">
         <v>45246</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>0.008699014111734016</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31">
         <v>0.01011935651271401</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="2" t="n">
+    <row r="32" spans="1:3">
+      <c r="A32" s="2">
         <v>45244</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>-0.01686469911843624</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32">
         <v>0.02452316076294281</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="2" t="n">
+    <row r="33" spans="1:3">
+      <c r="A33" s="2">
         <v>45243</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>0.03040935672514622</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33">
         <v>-0.002155243874133794</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="2" t="n">
+    <row r="34" spans="1:3">
+      <c r="A34" s="2">
         <v>45240</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>0.01002648505486192</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34">
         <v>0.01364568278829026</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="2" t="n">
+    <row r="35" spans="1:3">
+      <c r="A35" s="2">
         <v>45239</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>-0.02210151713804087</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35">
         <v>-0.0007304847227936895</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="2" t="n">
+    <row r="36" spans="1:3">
+      <c r="A36" s="2">
         <v>45238</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>0.0009576709442635778</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36">
         <v>-0.001416976892376853</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="2" t="n">
+    <row r="37" spans="1:3">
+      <c r="A37" s="2">
         <v>45237</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>-0.02659778032912363</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37">
         <v>0.006591440411184424</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="2" t="n">
+    <row r="38" spans="1:3">
+      <c r="A38" s="2">
         <v>45236</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>-0.003341851779044558</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38">
         <v>0.002767433987813206</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="2" t="n">
+    <row r="39" spans="1:3">
+      <c r="A39" s="2">
         <v>45233</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>-0.01400394477317557</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39">
         <v>0.02700494554683486</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="2" t="n">
+    <row r="40" spans="1:3">
+      <c r="A40" s="2">
         <v>45231</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>0.005601120224044909</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40">
         <v>0.0168723043201584</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="2" t="n">
+    <row r="41" spans="1:3">
+      <c r="A41" s="2">
         <v>45230</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>0.002387109608116056</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41">
         <v>0.005438453062240001</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="2" t="n">
+    <row r="42" spans="1:3">
+      <c r="A42" s="2">
         <v>45229</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>0.001587616590593255</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42">
         <v>-0.006787230474576522</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="2" t="n">
+    <row r="43" spans="1:3">
+      <c r="A43" s="2">
         <v>45226</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>0.005151575193184099</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43">
         <v>-0.01285971928173768</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="2" t="n">
+    <row r="44" spans="1:3">
+      <c r="A44" s="2">
         <v>45225</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>0.01517839542676924</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44">
         <v>0.0172560489231588</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="2" t="n">
+    <row r="45" spans="1:3">
+      <c r="A45" s="2">
         <v>45224</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>-0.002135922330097073</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45">
         <v>-0.008192542325205276</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="2" t="n">
+    <row r="46" spans="1:3">
+      <c r="A46" s="2">
         <v>45223</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>-0.001556723097878909</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46">
         <v>0.008662499445848404</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="2" t="n">
+    <row r="47" spans="1:3">
+      <c r="A47" s="2">
         <v>45222</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>0.03586045605145194</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47">
         <v>-0.00326985108921396</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="2" t="n">
+    <row r="48" spans="1:3">
+      <c r="A48" s="2">
         <v>45219</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>0.009219190968955848</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48">
         <v>-0.007447107119048502</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="2" t="n">
+    <row r="49" spans="1:3">
+      <c r="A49" s="2">
         <v>45218</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>0.01976137211036555</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49">
         <v>-0.0004909696650885476</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="2" t="n">
+    <row r="50" spans="1:3">
+      <c r="A50" s="2">
         <v>45217</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>0.001645338208409397</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50">
         <v>-0.01594367946992448</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="2" t="n">
+    <row r="51" spans="1:3">
+      <c r="A51" s="2">
         <v>45216</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>0.02482204781894515</v>
       </c>
-      <c r="C51" t="n">
+      <c r="C51">
         <v>-0.005371822815658955</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="2" t="n">
+    <row r="52" spans="1:3">
+      <c r="A52" s="2">
         <v>45215</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52">
         <v>-0.001602849510240367</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52">
         <v>0.006738428045683031</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="2" t="n">
+    <row r="53" spans="1:3">
+      <c r="A53" s="2">
         <v>45212</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>0.02069211559043871</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C53">
         <v>-0.01108064006287857</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" s="2" t="n">
+    <row r="54" spans="1:3">
+      <c r="A54" s="2">
         <v>45210</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54">
         <v>-0.03268088081090526</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54">
         <v>0.002689807002064448</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" s="2" t="n">
+    <row r="55" spans="1:3">
+      <c r="A55" s="2">
         <v>45209</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55">
         <v>-0.003432700993676652</v>
       </c>
-      <c r="C55" t="n">
+      <c r="C55">
         <v>0.01372920212581197</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="2" t="n">
+    <row r="56" spans="1:3">
+      <c r="A56" s="2">
         <v>45208</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B56">
         <v>0.00435097897026826</v>
       </c>
-      <c r="C56" t="n">
+      <c r="C56">
         <v>0.008636244197249621</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" s="2" t="n">
+    <row r="57" spans="1:3">
+      <c r="A57" s="2">
         <v>45205</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57">
         <v>-0.008844765342960303</v>
       </c>
-      <c r="C57" t="n">
+      <c r="C57">
         <v>0.007821051516542443</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="2" t="n">
+    <row r="58" spans="1:3">
+      <c r="A58" s="2">
         <v>45204</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58">
         <v>-0.01675468949189574</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C58">
         <v>-0.002843134665997726</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="2" t="n">
+    <row r="59" spans="1:3">
+      <c r="A59" s="2">
         <v>45203</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B59">
         <v>-0.004630487127245786</v>
       </c>
-      <c r="C59" t="n">
+      <c r="C59">
         <v>0.001657570601045766</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="2" t="n">
+    <row r="60" spans="1:3">
+      <c r="A60" s="2">
         <v>45202</v>
       </c>
-      <c r="B60" t="n">
+      <c r="B60">
         <v>0.005024190547078478</v>
       </c>
-      <c r="C60" t="n">
+      <c r="C60">
         <v>-0.01423642194738262</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="2" t="n">
+    <row r="61" spans="1:3">
+      <c r="A61" s="2">
         <v>45201</v>
       </c>
-      <c r="B61" t="n">
+      <c r="B61">
         <v>-0.01907054249213114</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C61">
         <v>-0.01293698794663922</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="2" t="n">
+    <row r="62" spans="1:3">
+      <c r="A62" s="2">
         <v>45198</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B62">
         <v>0.001132502831257209</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C62">
         <v>0.007206366487803706</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" s="2" t="n">
+    <row r="63" spans="1:3">
+      <c r="A63" s="2">
         <v>45197</v>
       </c>
-      <c r="B63" t="n">
+      <c r="B63">
         <v>-0.008295625942684737</v>
       </c>
-      <c r="C63" t="n">
+      <c r="C63">
         <v>0.01228056364638275</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="2" t="n">
+    <row r="64" spans="1:3">
+      <c r="A64" s="2">
         <v>45196</v>
       </c>
-      <c r="B64" t="n">
+      <c r="B64">
         <v>0.004372623574144363</v>
       </c>
-      <c r="C64" t="n">
+      <c r="C64">
         <v>0.00117345196290497</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" s="2" t="n">
+    <row r="65" spans="1:3">
+      <c r="A65" s="2">
         <v>45195</v>
       </c>
-      <c r="B65" t="n">
+      <c r="B65">
         <v>0.005300018928638961</v>
       </c>
-      <c r="C65" t="n">
+      <c r="C65">
         <v>-0.01494069441449208</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" s="2" t="n">
+    <row r="66" spans="1:3">
+      <c r="A66" s="2">
         <v>45194</v>
       </c>
-      <c r="B66" t="n">
+      <c r="B66">
         <v>0.015627942007155</v>
       </c>
-      <c r="C66" t="n">
+      <c r="C66">
         <v>-0.0007240817522778942</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="2" t="n">
+    <row r="67" spans="1:3">
+      <c r="A67" s="2">
         <v>45191</v>
       </c>
-      <c r="B67" t="n">
+      <c r="B67">
         <v>0.003151649981461002</v>
       </c>
-      <c r="C67" t="n">
+      <c r="C67">
         <v>-0.001170950105471635</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" s="2" t="n">
+    <row r="68" spans="1:3">
+      <c r="A68" s="2">
         <v>45190</v>
       </c>
-      <c r="B68" t="n">
+      <c r="B68">
         <v>0.0114581408242469</v>
       </c>
-      <c r="C68" t="n">
+      <c r="C68">
         <v>-0.02148363452546442</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" s="2" t="n">
+    <row r="69" spans="1:3">
+      <c r="A69" s="2">
         <v>45189</v>
       </c>
-      <c r="B69" t="n">
+      <c r="B69">
         <v>-0.02009866617942613</v>
       </c>
-      <c r="C69" t="n">
+      <c r="C69">
         <v>0.007204317499108992</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" s="2" t="n">
+    <row r="70" spans="1:3">
+      <c r="A70" s="2">
         <v>45188</v>
       </c>
-      <c r="B70" t="n">
+      <c r="B70">
         <v>-0.0384113369382808</v>
       </c>
-      <c r="C70" t="n">
+      <c r="C70">
         <v>-0.003736642770188037</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" s="2" t="n">
+    <row r="71" spans="1:3">
+      <c r="A71" s="2">
         <v>45187</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B71">
         <v>-0.0137676943959667</v>
       </c>
-      <c r="C71" t="n">
+      <c r="C71">
         <v>-0.003957628117684742</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="2" t="n">
+    <row r="72" spans="1:3">
+      <c r="A72" s="2">
         <v>45184</v>
       </c>
-      <c r="B72" t="n">
+      <c r="B72">
         <v>0.009241053873377814</v>
       </c>
-      <c r="C72" t="n">
+      <c r="C72">
         <v>-0.0053102385419459</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" s="2" t="n">
+    <row r="73" spans="1:3">
+      <c r="A73" s="2">
         <v>45183</v>
       </c>
-      <c r="B73" t="n">
+      <c r="B73">
         <v>-0.02474186635495801</v>
       </c>
-      <c r="C73" t="n">
+      <c r="C73">
         <v>0.01028973734091521</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="2" t="n">
+    <row r="74" spans="1:3">
+      <c r="A74" s="2">
         <v>45182</v>
       </c>
-      <c r="B74" t="n">
+      <c r="B74">
         <v>-0.0191769876148622</v>
       </c>
-      <c r="C74" t="n">
+      <c r="C74">
         <v>0.00176319001763181</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" s="2" t="n">
+    <row r="75" spans="1:3">
+      <c r="A75" s="2">
         <v>45181</v>
       </c>
-      <c r="B75" t="n">
+      <c r="B75">
         <v>0.0004073319755599769</v>
       </c>
-      <c r="C75" t="n">
+      <c r="C75">
         <v>0.009282787060564734</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="2" t="n">
+    <row r="76" spans="1:3">
+      <c r="A76" s="2">
         <v>45180</v>
       </c>
-      <c r="B76" t="n">
+      <c r="B76">
         <v>-0.006107491856677472</v>
       </c>
-      <c r="C76" t="n">
+      <c r="C76">
         <v>0.01361511711602326</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="2" t="n">
+    <row r="77" spans="1:3">
+      <c r="A77" s="2">
         <v>45177</v>
       </c>
-      <c r="B77" t="n">
+      <c r="B77">
         <v>-0.02693877551020407</v>
       </c>
-      <c r="C77" t="n">
+      <c r="C77">
         <v>-0.005793852653360299</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="2" t="n">
+    <row r="78" spans="1:3">
+      <c r="A78" s="2">
         <v>45175</v>
       </c>
-      <c r="B78" t="n">
+      <c r="B78">
         <v>0.02181208053691264</v>
       </c>
-      <c r="C78" t="n">
+      <c r="C78">
         <v>-0.0114718190418559</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="2" t="n">
+    <row r="79" spans="1:3">
+      <c r="A79" s="2">
         <v>45174</v>
       </c>
-      <c r="B79" t="n">
+      <c r="B79">
         <v>0.01621510673234816</v>
       </c>
-      <c r="C79" t="n">
+      <c r="C79">
         <v>-0.003786817460115333</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="2" t="n">
+    <row r="80" spans="1:3">
+      <c r="A80" s="2">
         <v>45173</v>
       </c>
-      <c r="B80" t="n">
+      <c r="B80">
         <v>0.005857402544940493</v>
       </c>
-      <c r="C80" t="n">
+      <c r="C80">
         <v>-0.0009839430670184335</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="2" t="n">
+    <row r="81" spans="1:3">
+      <c r="A81" s="2">
         <v>45170</v>
       </c>
-      <c r="B81" t="n">
+      <c r="B81">
         <v>-0.02385141739980445</v>
       </c>
-      <c r="C81" t="n">
+      <c r="C81">
         <v>0.01858443780131669</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" s="2" t="n">
+    <row r="82" spans="1:3">
+      <c r="A82" s="2">
         <v>45169</v>
       </c>
-      <c r="B82" t="n">
+      <c r="B82">
         <v>-0.0186260765071099</v>
       </c>
-      <c r="C82" t="n">
+      <c r="C82">
         <v>-0.01525503041647169</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="2" t="n">
+    <row r="83" spans="1:3">
+      <c r="A83" s="2">
         <v>45168</v>
       </c>
-      <c r="B83" t="n">
+      <c r="B83">
         <v>0.01367346938775515</v>
       </c>
-      <c r="C83" t="n">
+      <c r="C83">
         <v>-0.007339279078409477</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" s="2" t="n">
+    <row r="84" spans="1:3">
+      <c r="A84" s="2">
         <v>45167</v>
       </c>
-      <c r="B84" t="n">
+      <c r="B84">
         <v>0.006241191866317664</v>
       </c>
-      <c r="C84" t="n">
+      <c r="C84">
         <v>0.01095448297060297</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" s="2" t="n">
+    <row r="85" spans="1:3">
+      <c r="A85" s="2">
         <v>45166</v>
       </c>
-      <c r="B85" t="n">
+      <c r="B85">
         <v>-0.0166066426570628</v>
       </c>
-      <c r="C85" t="n">
+      <c r="C85">
         <v>0.01108454120876745</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="2" t="n">
+    <row r="86" spans="1:3">
+      <c r="A86" s="2">
         <v>45163</v>
       </c>
-      <c r="B86" t="n">
+      <c r="B86">
         <v>-0.007934893184130209</v>
       </c>
-      <c r="C86" t="n">
+      <c r="C86">
         <v>-0.01016013535453664</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" s="2" t="n">
+    <row r="87" spans="1:3">
+      <c r="A87" s="2">
         <v>45162</v>
       </c>
-      <c r="B87" t="n">
+      <c r="B87">
         <v>-0.01107465135356844</v>
       </c>
-      <c r="C87" t="n">
+      <c r="C87">
         <v>-0.009387565073856186</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="2" t="n">
+    <row r="88" spans="1:3">
+      <c r="A88" s="2">
         <v>45161</v>
       </c>
-      <c r="B88" t="n">
+      <c r="B88">
         <v>0.002695976773123165</v>
       </c>
-      <c r="C88" t="n">
+      <c r="C88">
         <v>0.01703743241847167</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" s="2" t="n">
+    <row r="89" spans="1:3">
+      <c r="A89" s="2">
         <v>45160</v>
       </c>
-      <c r="B89" t="n">
+      <c r="B89">
         <v>0.007445708376421889</v>
       </c>
-      <c r="C89" t="n">
+      <c r="C89">
         <v>0.0150923279937778</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" s="2" t="n">
+    <row r="90" spans="1:3">
+      <c r="A90" s="2">
         <v>45159</v>
       </c>
-      <c r="B90" t="n">
+      <c r="B90">
         <v>0.004516526380619945</v>
       </c>
-      <c r="C90" t="n">
+      <c r="C90">
         <v>-0.008491538788136133</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" s="2" t="n">
+    <row r="91" spans="1:3">
+      <c r="A91" s="2">
         <v>45156</v>
       </c>
-      <c r="B91" t="n">
+      <c r="B91">
         <v>0.01205804210096062</v>
       </c>
-      <c r="C91" t="n">
+      <c r="C91">
         <v>0.00371362474126391</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" s="2" t="n">
+    <row r="92" spans="1:3">
+      <c r="A92" s="2">
         <v>45155</v>
       </c>
-      <c r="B92" t="n">
+      <c r="B92">
         <v>-0.005452342487883732</v>
       </c>
-      <c r="C92" t="n">
+      <c r="C92">
         <v>-0.005277181811890075</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" s="2" t="n">
+    <row r="93" spans="1:3">
+      <c r="A93" s="2">
         <v>45154</v>
       </c>
-      <c r="B93" t="n">
+      <c r="B93">
         <v>-0.009746192893400951</v>
       </c>
-      <c r="C93" t="n">
+      <c r="C93">
         <v>-0.00498403215948906</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" s="2" t="n">
+    <row r="94" spans="1:3">
+      <c r="A94" s="2">
         <v>45153</v>
       </c>
-      <c r="B94" t="n">
+      <c r="B94">
         <v>0.002460529013737833</v>
       </c>
-      <c r="C94" t="n">
+      <c r="C94">
         <v>-0.005470422052906376</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" s="2" t="n">
+    <row r="95" spans="1:3">
+      <c r="A95" s="2">
         <v>45152</v>
       </c>
-      <c r="B95" t="n">
+      <c r="B95">
         <v>0.01759050930660666</v>
       </c>
-      <c r="C95" t="n">
+      <c r="C95">
         <v>-0.01062973785626564</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" s="2" t="n">
+    <row r="96" spans="1:3">
+      <c r="A96" s="2">
         <v>45149</v>
       </c>
-      <c r="B96" t="n">
+      <c r="B96">
         <v>-0.01467336683417075</v>
       </c>
-      <c r="C96" t="n">
+      <c r="C96">
         <v>-0.002408111533586776</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" s="2" t="n">
+    <row r="97" spans="1:3">
+      <c r="A97" s="2">
         <v>45148</v>
       </c>
-      <c r="B97" t="n">
+      <c r="B97">
         <v>-0.01631986944104458</v>
       </c>
-      <c r="C97" t="n">
+      <c r="C97">
         <v>-0.0004982729353343318</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" s="2" t="n">
+    <row r="98" spans="1:3">
+      <c r="A98" s="2">
         <v>45147</v>
       </c>
-      <c r="B98" t="n">
+      <c r="B98">
         <v>-0.001036914143508816</v>
       </c>
-      <c r="C98" t="n">
+      <c r="C98">
         <v>-0.005718364262322639</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" s="2" t="n">
+    <row r="99" spans="1:3">
+      <c r="A99" s="2">
         <v>45146</v>
       </c>
-      <c r="B99" t="n">
+      <c r="B99">
         <v>0.009134315964293149</v>
       </c>
-      <c r="C99" t="n">
+      <c r="C99">
         <v>-0.002429217624392743</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" s="2" t="n">
+    <row r="100" spans="1:3">
+      <c r="A100" s="2">
         <v>45145</v>
       </c>
-      <c r="B100" t="n">
+      <c r="B100">
         <v>0.01542892408969343</v>
       </c>
-      <c r="C100" t="n">
+      <c r="C100">
         <v>-0.001071058004485037</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" s="2" t="n">
+    <row r="101" spans="1:3">
+      <c r="A101" s="2">
         <v>45142</v>
       </c>
-      <c r="B101" t="n">
+      <c r="B101">
         <v>-0.004862236628849326</v>
       </c>
-      <c r="C101" t="n">
+      <c r="C101">
         <v>-0.00893967790622463</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" s="2" t="n">
+    <row r="102" spans="1:3">
+      <c r="A102" s="2">
         <v>45141</v>
       </c>
-      <c r="B102" t="n">
+      <c r="B102">
         <v>-0.0126221498371335</v>
       </c>
-      <c r="C102" t="n">
+      <c r="C102">
         <v>-0.002258830538064971</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" s="2" t="n">
+    <row r="103" spans="1:3">
+      <c r="A103" s="2">
         <v>45140</v>
       </c>
-      <c r="B103" t="n">
+      <c r="B103">
         <v>-0.03525773195876292</v>
       </c>
-      <c r="C103" t="n">
+      <c r="C103">
         <v>-0.003208300343098491</v>
       </c>
     </row>
-    <row r="104">
-      <c r="A104" s="2" t="n">
+    <row r="104" spans="1:3">
+      <c r="A104" s="2">
         <v>45139</v>
       </c>
-      <c r="B104" t="n">
+      <c r="B104">
         <v>0.0102586022654414</v>
       </c>
-      <c r="C104" t="n">
+      <c r="C104">
         <v>-0.005699384138490915</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" s="2" t="n">
+    <row r="105" spans="1:3">
+      <c r="A105" s="2">
         <v>45138</v>
       </c>
-      <c r="B105" t="n">
+      <c r="B105">
         <v>-0.006346519991538013</v>
       </c>
-      <c r="C105" t="n">
+      <c r="C105">
         <v>0.01461056520255943</v>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" s="2" t="n">
+    <row r="106" spans="1:3">
+      <c r="A106" s="2">
         <v>45135</v>
       </c>
-      <c r="B106" t="n">
+      <c r="B106">
         <v>-0.0178837555886735</v>
       </c>
-      <c r="C106" t="n">
+      <c r="C106">
         <v>0.001641803483623638</v>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" s="2" t="n">
+    <row r="107" spans="1:3">
+      <c r="A107" s="2">
         <v>45134</v>
       </c>
-      <c r="B107" t="n">
+      <c r="B107">
         <v>-0.0002167786689790674</v>
       </c>
-      <c r="C107" t="n">
+      <c r="C107">
         <v>-0.0209693211488251</v>
       </c>
     </row>
-    <row r="108">
-      <c r="A108" s="2" t="n">
+    <row r="108" spans="1:3">
+      <c r="A108" s="2">
         <v>45133</v>
       </c>
-      <c r="B108" t="n">
+      <c r="B108">
         <v>-0.01539462272333048</v>
       </c>
-      <c r="C108" t="n">
+      <c r="C108">
         <v>0.004524293488951558</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" s="2" t="n">
+    <row r="109" spans="1:3">
+      <c r="A109" s="2">
         <v>45132</v>
       </c>
-      <c r="B109" t="n">
+      <c r="B109">
         <v>-0.02686632900242236</v>
       </c>
-      <c r="C109" t="n">
+      <c r="C109">
         <v>0.005488618944800683</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" s="2" t="n">
+    <row r="110" spans="1:3">
+      <c r="A110" s="2">
         <v>45131</v>
       </c>
-      <c r="B110" t="n">
+      <c r="B110">
         <v>-0.004525910839556335</v>
       </c>
-      <c r="C110" t="n">
+      <c r="C110">
         <v>0.009358077476563142</v>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" s="2" t="n">
+    <row r="111" spans="1:3">
+      <c r="A111" s="2">
         <v>45128</v>
       </c>
-      <c r="B111" t="n">
+      <c r="B111">
         <v>-0.02136849283928177</v>
       </c>
-      <c r="C111" t="n">
+      <c r="C111">
         <v>0.01807203407772495</v>
       </c>
     </row>
-    <row r="112">
-      <c r="A112" s="2" t="n">
+    <row r="112" spans="1:3">
+      <c r="A112" s="2">
         <v>45127</v>
       </c>
-      <c r="B112" t="n">
+      <c r="B112">
         <v>-0.009291521486643362</v>
       </c>
-      <c r="C112" t="n">
+      <c r="C112">
         <v>0.004517149857084624</v>
       </c>
     </row>
-    <row r="113">
-      <c r="A113" s="2" t="n">
+    <row r="113" spans="1:3">
+      <c r="A113" s="2">
         <v>45126</v>
       </c>
-      <c r="B113" t="n">
+      <c r="B113">
         <v>-0.004220398593200447</v>
       </c>
-      <c r="C113" t="n">
+      <c r="C113">
         <v>-0.002452457124430429</v>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" s="2" t="n">
+    <row r="114" spans="1:3">
+      <c r="A114" s="2">
         <v>45125</v>
       </c>
-      <c r="B114" t="n">
+      <c r="B114">
         <v>0.02542971509300673</v>
       </c>
-      <c r="C114" t="n">
+      <c r="C114">
         <v>-0.003197455569747709</v>
       </c>
     </row>
-    <row r="115">
-      <c r="A115" s="2" t="n">
+    <row r="115" spans="1:3">
+      <c r="A115" s="2">
         <v>45124</v>
       </c>
-      <c r="B115" t="n">
+      <c r="B115">
         <v>-0.00390355912743956</v>
       </c>
-      <c r="C115" t="n">
+      <c r="C115">
         <v>0.004315654441810812</v>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" s="2" t="n">
+    <row r="116" spans="1:3">
+      <c r="A116" s="2">
         <v>45121</v>
       </c>
-      <c r="B116" t="n">
+      <c r="B116">
         <v>0.003457814661134151</v>
       </c>
-      <c r="C116" t="n">
+      <c r="C116">
         <v>-0.01302153206332168</v>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" s="2" t="n">
+    <row r="117" spans="1:3">
+      <c r="A117" s="2">
         <v>45120</v>
       </c>
-      <c r="B117" t="n">
+      <c r="B117">
         <v>-0.004135079255685681</v>
       </c>
-      <c r="C117" t="n">
+      <c r="C117">
         <v>0.01358081348902829</v>
       </c>
     </row>
-    <row r="118">
-      <c r="A118" s="2" t="n">
+    <row r="118" spans="1:3">
+      <c r="A118" s="2">
         <v>45119</v>
       </c>
-      <c r="B118" t="n">
+      <c r="B118">
         <v>-0.004152249134948049</v>
       </c>
-      <c r="C118" t="n">
+      <c r="C118">
         <v>0.003804811465620173</v>
       </c>
     </row>
-    <row r="119">
-      <c r="A119" s="2" t="n">
+    <row r="119" spans="1:3">
+      <c r="A119" s="2">
         <v>45118</v>
       </c>
-      <c r="B119" t="n">
+      <c r="B119">
         <v>-0.003011350474866892</v>
       </c>
-      <c r="C119" t="n">
+      <c r="C119">
         <v>-0.006121653015889184</v>
       </c>
     </row>
-    <row r="120">
-      <c r="A120" s="2" t="n">
+    <row r="120" spans="1:3">
+      <c r="A120" s="2">
         <v>45117</v>
       </c>
-      <c r="B120" t="n">
+      <c r="B120">
         <v>-0.0004646840148697651</v>
       </c>
-      <c r="C120" t="n">
+      <c r="C120">
         <v>-0.008040505307069901</v>
       </c>
     </row>
-    <row r="121">
-      <c r="A121" s="2" t="n">
+    <row r="121" spans="1:3">
+      <c r="A121" s="2">
         <v>45114</v>
       </c>
-      <c r="B121" t="n">
+      <c r="B121">
         <v>0.01092515109251502</v>
       </c>
-      <c r="C121" t="n">
+      <c r="C121">
         <v>0.01253555430654196</v>
       </c>
     </row>
-    <row r="122">
-      <c r="A122" s="2" t="n">
+    <row r="122" spans="1:3">
+      <c r="A122" s="2">
         <v>45113</v>
       </c>
-      <c r="B122" t="n">
+      <c r="B122">
         <v>-0.008967578753736549</v>
       </c>
-      <c r="C122" t="n">
+      <c r="C122">
         <v>-0.01775840868597811</v>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" s="2" t="n">
+    <row r="123" spans="1:3">
+      <c r="A123" s="2">
         <v>45112</v>
       </c>
-      <c r="B123" t="n">
+      <c r="B123">
         <v>0.007656612529002293</v>
       </c>
-      <c r="C123" t="n">
+      <c r="C123">
         <v>0.003972253014881355</v>
       </c>
     </row>
-    <row r="124">
-      <c r="A124" s="2" t="n">
+    <row r="124" spans="1:3">
+      <c r="A124" s="2">
         <v>45111</v>
       </c>
-      <c r="B124" t="n">
+      <c r="B124">
         <v>0.006447156343541316</v>
       </c>
-      <c r="C124" t="n">
+      <c r="C124">
         <v>-0.004988593918427764</v>
       </c>
     </row>
-    <row r="125">
-      <c r="A125" s="2" t="n">
+    <row r="125" spans="1:3">
+      <c r="A125" s="2">
         <v>45110</v>
       </c>
-      <c r="B125" t="n">
+      <c r="B125">
         <v>-0.01143902997025847</v>
       </c>
-      <c r="C125" t="n">
+      <c r="C125">
         <v>0.01343077561458927</v>
       </c>
     </row>
-    <row r="126">
-      <c r="A126" s="2" t="n">
+    <row r="126" spans="1:3">
+      <c r="A126" s="2">
         <v>45107</v>
       </c>
-      <c r="B126" t="n">
+      <c r="B126">
         <v>0</v>
       </c>
-      <c r="C126" t="n">
+      <c r="C126">
         <v>-0.002500359004248942</v>
       </c>
     </row>
-    <row r="127">
-      <c r="A127" s="2" t="n">
+    <row r="127" spans="1:3">
+      <c r="A127" s="2">
         <v>45106</v>
       </c>
-      <c r="B127" t="n">
+      <c r="B127">
         <v>-0.003934274473501587</v>
       </c>
-      <c r="C127" t="n">
+      <c r="C127">
         <v>0.01458677933853836</v>
       </c>
     </row>
-    <row r="128">
-      <c r="A128" s="2" t="n">
+    <row r="128" spans="1:3">
+      <c r="A128" s="2">
         <v>45105</v>
       </c>
-      <c r="B128" t="n">
+      <c r="B128">
         <v>0.002788104089219257</v>
       </c>
-      <c r="C128" t="n">
+      <c r="C128">
         <v>-0.007164555023272068</v>
       </c>
     </row>
-    <row r="129">
-      <c r="A129" s="2" t="n">
+    <row r="129" spans="1:3">
+      <c r="A129" s="2">
         <v>45104</v>
       </c>
-      <c r="B129" t="n">
+      <c r="B129">
         <v>0.01506024096385561</v>
       </c>
-      <c r="C129" t="n">
+      <c r="C129">
         <v>-0.006089155383405376</v>
       </c>
     </row>
-    <row r="130">
-      <c r="A130" s="2" t="n">
+    <row r="130" spans="1:3">
+      <c r="A130" s="2">
         <v>45103</v>
       </c>
-      <c r="B130" t="n">
+      <c r="B130">
         <v>0.01711937913718331</v>
       </c>
-      <c r="C130" t="n">
+      <c r="C130">
         <v>-0.006169259604797528</v>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" s="2" t="n">
+    <row r="131" spans="1:3">
+      <c r="A131" s="2">
         <v>45100</v>
       </c>
-      <c r="B131" t="n">
+      <c r="B131">
         <v>0.007405745062836644</v>
       </c>
-      <c r="C131" t="n">
+      <c r="C131">
         <v>0.0003615450586038627</v>
       </c>
     </row>
-    <row r="132">
-      <c r="A132" s="2" t="n">
+    <row r="132" spans="1:3">
+      <c r="A132" s="2">
         <v>45099</v>
       </c>
-      <c r="B132" t="n">
+      <c r="B132">
         <v>-0.00178213410559136</v>
       </c>
-      <c r="C132" t="n">
+      <c r="C132">
         <v>-0.01234014283341633</v>
       </c>
     </row>
-    <row r="133">
-      <c r="A133" s="2" t="n">
+    <row r="133" spans="1:3">
+      <c r="A133" s="2">
         <v>45098</v>
       </c>
-      <c r="B133" t="n">
+      <c r="B133">
         <v>0.01338986833296119</v>
       </c>
-      <c r="C133" t="n">
+      <c r="C133">
         <v>0.006671013693133387</v>
       </c>
     </row>
-    <row r="134">
-      <c r="A134" s="2" t="n">
+    <row r="134" spans="1:3">
+      <c r="A134" s="2">
         <v>45097</v>
       </c>
-      <c r="B134" t="n">
+      <c r="B134">
         <v>0.02070028628055498</v>
       </c>
-      <c r="C134" t="n">
+      <c r="C134">
         <v>-0.001968996646031118</v>
       </c>
     </row>
-    <row r="135">
-      <c r="A135" s="2" t="n">
+    <row r="135" spans="1:3">
+      <c r="A135" s="2">
         <v>45096</v>
       </c>
-      <c r="B135" t="n">
+      <c r="B135">
         <v>0.005609492988133624</v>
       </c>
-      <c r="C135" t="n">
+      <c r="C135">
         <v>0.009262533892453462</v>
       </c>
     </row>
-    <row r="136">
-      <c r="A136" s="2" t="n">
+    <row r="136" spans="1:3">
+      <c r="A136" s="2">
         <v>45093</v>
       </c>
-      <c r="B136" t="n">
+      <c r="B136">
         <v>0.01244368161338771</v>
       </c>
-      <c r="C136" t="n">
+      <c r="C136">
         <v>-0.003883544006508921</v>
       </c>
     </row>
-    <row r="137">
-      <c r="A137" s="2" t="n">
+    <row r="137" spans="1:3">
+      <c r="A137" s="2">
         <v>45092</v>
       </c>
-      <c r="B137" t="n">
+      <c r="B137">
         <v>0.0008476372112735664</v>
       </c>
-      <c r="C137" t="n">
+      <c r="C137">
         <v>0.001276570727897219</v>
       </c>
     </row>
-    <row r="138">
-      <c r="A138" s="2" t="n">
+    <row r="138" spans="1:3">
+      <c r="A138" s="2">
         <v>45091</v>
       </c>
-      <c r="B138" t="n">
+      <c r="B138">
         <v>-0.03493542240101633</v>
       </c>
-      <c r="C138" t="n">
+      <c r="C138">
         <v>0.01992410679869461</v>
       </c>
     </row>
-    <row r="139">
-      <c r="A139" s="2" t="n">
+    <row r="139" spans="1:3">
+      <c r="A139" s="2">
         <v>45090</v>
       </c>
-      <c r="B139" t="n">
+      <c r="B139">
         <v>0.008556384379113657</v>
       </c>
-      <c r="C139" t="n">
+      <c r="C139">
         <v>-0.005053862412217947</v>
       </c>
     </row>
-    <row r="140">
-      <c r="A140" s="2" t="n">
+    <row r="140" spans="1:3">
+      <c r="A140" s="2">
         <v>45089</v>
       </c>
-      <c r="B140" t="n">
+      <c r="B140">
         <v>-0.007396127909506167</v>
       </c>
-      <c r="C140" t="n">
+      <c r="C140">
         <v>0.00270896179252933</v>
       </c>
     </row>
-    <row r="141">
-      <c r="A141" s="2" t="n">
+    <row r="141" spans="1:3">
+      <c r="A141" s="2">
         <v>45086</v>
       </c>
-      <c r="B141" t="n">
+      <c r="B141">
         <v>-0.03133903133903138</v>
       </c>
-      <c r="C141" t="n">
+      <c r="C141">
         <v>0.01325678858409529</v>
       </c>
     </row>
-    <row r="142">
-      <c r="A142" s="2" t="n">
+    <row r="142" spans="1:3">
+      <c r="A142" s="2">
         <v>45084</v>
       </c>
-      <c r="B142" t="n">
+      <c r="B142">
         <v>0.01312217194570131</v>
       </c>
-      <c r="C142" t="n">
+      <c r="C142">
         <v>0.007660762586161773</v>
       </c>
     </row>
-    <row r="143">
-      <c r="A143" s="2" t="n">
+    <row r="143" spans="1:3">
+      <c r="A143" s="2">
         <v>45083</v>
       </c>
-      <c r="B143" t="n">
+      <c r="B143">
         <v>0.02411790978115236</v>
       </c>
-      <c r="C143" t="n">
+      <c r="C143">
         <v>0.0169837438773337</v>
       </c>
     </row>
-    <row r="144">
-      <c r="A144" s="2" t="n">
+    <row r="144" spans="1:3">
+      <c r="A144" s="2">
         <v>45082</v>
       </c>
-      <c r="B144" t="n">
+      <c r="B144">
         <v>-0.002616659398168242</v>
       </c>
-      <c r="C144" t="n">
+      <c r="C144">
         <v>0.001226034577728852</v>
       </c>
     </row>
-    <row r="145">
-      <c r="A145" s="2" t="n">
+    <row r="145" spans="1:3">
+      <c r="A145" s="2">
         <v>45079</v>
       </c>
-      <c r="B145" t="n">
+      <c r="B145">
         <v>-0.008307826847398392</v>
       </c>
-      <c r="C145" t="n">
+      <c r="C145">
         <v>0.01802559580337348</v>
       </c>
     </row>
-    <row r="146">
-      <c r="A146" s="2" t="n">
+    <row r="146" spans="1:3">
+      <c r="A146" s="2">
         <v>45078</v>
       </c>
-      <c r="B146" t="n">
+      <c r="B146">
         <v>-0.03064373897707229</v>
       </c>
-      <c r="C146" t="n">
+      <c r="C146">
         <v>0.02058429870309686</v>
       </c>
     </row>
-    <row r="147">
-      <c r="A147" s="2" t="n">
+    <row r="147" spans="1:3">
+      <c r="A147" s="2">
         <v>45077</v>
       </c>
-      <c r="B147" t="n">
+      <c r="B147">
         <v>-0.005003411416875103</v>
       </c>
-      <c r="C147" t="n">
+      <c r="C147">
         <v>-0.005799921077023318</v>
       </c>
     </row>
-    <row r="148">
-      <c r="A148" s="2" t="n">
+    <row r="148" spans="1:3">
+      <c r="A148" s="2">
         <v>45076</v>
       </c>
-      <c r="B148" t="n">
+      <c r="B148">
         <v>0.00777142857142854</v>
       </c>
-      <c r="C148" t="n">
+      <c r="C148">
         <v>-0.01238070205650166</v>
       </c>
     </row>
-    <row r="149">
-      <c r="A149" s="2" t="n">
+    <row r="149" spans="1:3">
+      <c r="A149" s="2">
         <v>45075</v>
       </c>
-      <c r="B149" t="n">
+      <c r="B149">
         <v>0.005670220004536208</v>
       </c>
-      <c r="C149" t="n">
+      <c r="C149">
         <v>-0.005166537428092255</v>
       </c>
     </row>
-    <row r="150">
-      <c r="A150" s="2" t="n">
+    <row r="150" spans="1:3">
+      <c r="A150" s="2">
         <v>45072</v>
       </c>
-      <c r="B150" t="n">
+      <c r="B150">
         <v>-0.0006765899864682456</v>
       </c>
-      <c r="C150" t="n">
+      <c r="C150">
         <v>0.007741654097079609</v>
       </c>
     </row>
-    <row r="151">
-      <c r="A151" s="2" t="n">
+    <row r="151" spans="1:3">
+      <c r="A151" s="2">
         <v>45071</v>
       </c>
-      <c r="B151" t="n">
+      <c r="B151">
         <v>-0.02708192281652</v>
       </c>
-      <c r="C151" t="n">
+      <c r="C151">
         <v>0.0115257352941176</v>
       </c>
     </row>
-    <row r="152">
-      <c r="A152" s="2" t="n">
+    <row r="152" spans="1:3">
+      <c r="A152" s="2">
         <v>45070</v>
       </c>
-      <c r="B152" t="n">
+      <c r="B152">
         <v>0.01067037810252836</v>
       </c>
-      <c r="C152" t="n">
+      <c r="C152">
         <v>-0.0102702653530915</v>
       </c>
     </row>
-    <row r="153">
-      <c r="A153" s="2" t="n">
+    <row r="153" spans="1:3">
+      <c r="A153" s="2">
         <v>45069</v>
       </c>
-      <c r="B153" t="n">
+      <c r="B153">
         <v>0.02845994950654118</v>
       </c>
-      <c r="C153" t="n">
+      <c r="C153">
         <v>-0.00257682850480434</v>
       </c>
     </row>
-    <row r="154">
-      <c r="A154" s="2" t="n">
+    <row r="154" spans="1:3">
+      <c r="A154" s="2">
         <v>45068</v>
       </c>
-      <c r="B154" t="n">
+      <c r="B154">
         <v>-0.01495201963847359</v>
       </c>
-      <c r="C154" t="n">
+      <c r="C154">
         <v>-0.004803828615287387</v>
       </c>
     </row>
-    <row r="155">
-      <c r="A155" s="2" t="n">
+    <row r="155" spans="1:3">
+      <c r="A155" s="2">
         <v>45065</v>
       </c>
-      <c r="B155" t="n">
+      <c r="B155">
         <v>0.005437245129134682</v>
       </c>
-      <c r="C155" t="n">
+      <c r="C155">
         <v>0.005785229047843954</v>
       </c>
     </row>
-    <row r="156">
-      <c r="A156" s="2" t="n">
+    <row r="156" spans="1:3">
+      <c r="A156" s="2">
         <v>45064</v>
       </c>
-      <c r="B156" t="n">
+      <c r="B156">
         <v>-0.001577287066246047</v>
       </c>
-      <c r="C156" t="n">
+      <c r="C156">
         <v>0.005919970765576377</v>
       </c>
     </row>
-    <row r="157">
-      <c r="A157" s="2" t="n">
+    <row r="157" spans="1:3">
+      <c r="A157" s="2">
         <v>45063</v>
       </c>
-      <c r="B157" t="n">
+      <c r="B157">
         <v>-0.03565786504175139</v>
       </c>
-      <c r="C157" t="n">
+      <c r="C157">
         <v>0.01170120339390346</v>
       </c>
     </row>
-    <row r="158">
-      <c r="A158" s="2" t="n">
+    <row r="158" spans="1:3">
+      <c r="A158" s="2">
         <v>45062</v>
       </c>
-      <c r="B158" t="n">
+      <c r="B158">
         <v>-0.0004680552305170727</v>
       </c>
-      <c r="C158" t="n">
+      <c r="C158">
         <v>-0.007658512872721901</v>
       </c>
     </row>
-    <row r="159">
-      <c r="A159" s="2" t="n">
+    <row r="159" spans="1:3">
+      <c r="A159" s="2">
         <v>45061</v>
       </c>
-      <c r="B159" t="n">
+      <c r="B159">
         <v>-0.01826270194333879</v>
       </c>
-      <c r="C159" t="n">
+      <c r="C159">
         <v>0.005209101637409619</v>
       </c>
     </row>
-    <row r="160">
-      <c r="A160" s="2" t="n">
+    <row r="160" spans="1:3">
+      <c r="A160" s="2">
         <v>45058</v>
       </c>
-      <c r="B160" t="n">
+      <c r="B160">
         <v>-0.01097066539470548</v>
       </c>
-      <c r="C160" t="n">
+      <c r="C160">
         <v>0.001921371563700758</v>
       </c>
     </row>
-    <row r="161">
-      <c r="A161" s="2" t="n">
+    <row r="161" spans="1:3">
+      <c r="A161" s="2">
         <v>45057</v>
       </c>
-      <c r="B161" t="n">
+      <c r="B161">
         <v>-0.02049674463467566</v>
       </c>
-      <c r="C161" t="n">
+      <c r="C161">
         <v>0.007519916610825739</v>
       </c>
     </row>
-    <row r="162">
-      <c r="A162" s="2" t="n">
+    <row r="162" spans="1:3">
+      <c r="A162" s="2">
         <v>45056</v>
       </c>
-      <c r="B162" t="n">
+      <c r="B162">
         <v>0.002708025603151087</v>
       </c>
-      <c r="C162" t="n">
+      <c r="C162">
         <v>0.003118173161304805</v>
       </c>
     </row>
-    <row r="163">
-      <c r="A163" s="2" t="n">
+    <row r="163" spans="1:3">
+      <c r="A163" s="2">
         <v>45055</v>
       </c>
-      <c r="B163" t="n">
+      <c r="B163">
         <v>-0.004419346918733136</v>
       </c>
-      <c r="C163" t="n">
+      <c r="C163">
         <v>0.01010920201429633</v>
       </c>
     </row>
-    <row r="164">
-      <c r="A164" s="2" t="n">
+    <row r="164" spans="1:3">
+      <c r="A164" s="2">
         <v>45054</v>
       </c>
-      <c r="B164" t="n">
+      <c r="B164">
         <v>0.008877928483353781</v>
       </c>
-      <c r="C164" t="n">
+      <c r="C164">
         <v>0.008502301517860467</v>
       </c>
     </row>
-    <row r="165">
-      <c r="A165" s="2" t="n">
+    <row r="165" spans="1:3">
+      <c r="A165" s="2">
         <v>45051</v>
       </c>
-      <c r="B165" t="n">
+      <c r="B165">
         <v>-0.02587446094873036</v>
       </c>
-      <c r="C165" t="n">
+      <c r="C165">
         <v>0.02910720927046029</v>
       </c>
     </row>
-    <row r="166">
-      <c r="A166" s="2" t="n">
+    <row r="166" spans="1:3">
+      <c r="A166" s="2">
         <v>45050</v>
       </c>
-      <c r="B166" t="n">
+      <c r="B166">
         <v>-0.04845056566650263</v>
       </c>
-      <c r="C166" t="n">
+      <c r="C166">
         <v>0.003703449021090988</v>
       </c>
     </row>
-    <row r="167">
-      <c r="A167" s="2" t="n">
+    <row r="167" spans="1:3">
+      <c r="A167" s="2">
         <v>45049</v>
       </c>
-      <c r="B167" t="n">
+      <c r="B167">
         <v>0.01266477125872334</v>
       </c>
-      <c r="C167" t="n">
+      <c r="C167">
         <v>-0.001275422606375143</v>
       </c>
     </row>
-    <row r="168">
-      <c r="A168" s="2" t="n">
+    <row r="168" spans="1:3">
+      <c r="A168" s="2">
         <v>45048</v>
       </c>
-      <c r="B168" t="n">
+      <c r="B168">
         <v>0.01454823889739654</v>
       </c>
-      <c r="C168" t="n">
+      <c r="C168">
         <v>-0.02398690056687602</v>
       </c>
     </row>
-    <row r="169">
-      <c r="A169" s="2" t="n">
+    <row r="169" spans="1:3">
+      <c r="A169" s="2">
         <v>45044</v>
       </c>
-      <c r="B169" t="n">
+      <c r="B169">
         <v>-0.02163522012578611</v>
       </c>
-      <c r="C169" t="n">
+      <c r="C169">
         <v>0.01466144593531093</v>
       </c>
     </row>
-    <row r="170">
-      <c r="A170" s="2" t="n">
+    <row r="170" spans="1:3">
+      <c r="A170" s="2">
         <v>45043</v>
       </c>
-      <c r="B170" t="n">
+      <c r="B170">
         <v>-0.04525584983286191</v>
       </c>
-      <c r="C170" t="n">
+      <c r="C170">
         <v>0.005971929001485687</v>
       </c>
     </row>
-    <row r="171">
-      <c r="A171" s="2" t="n">
+    <row r="171" spans="1:3">
+      <c r="A171" s="2">
         <v>45042</v>
       </c>
-      <c r="B171" t="n">
+      <c r="B171">
         <v>0.00673309991920279</v>
       </c>
-      <c r="C171" t="n">
+      <c r="C171">
         <v>-0.008796744816895963</v>
       </c>
     </row>
-    <row r="172">
-      <c r="A172" s="2" t="n">
+    <row r="172" spans="1:3">
+      <c r="A172" s="2">
         <v>45041</v>
       </c>
-      <c r="B172" t="n">
+      <c r="B172">
         <v>0.01417870518994091</v>
       </c>
-      <c r="C172" t="n">
+      <c r="C172">
         <v>-0.006993948839312369</v>
       </c>
     </row>
-    <row r="173">
-      <c r="A173" s="2" t="n">
+    <row r="173" spans="1:3">
+      <c r="A173" s="2">
         <v>45040</v>
       </c>
-      <c r="B173" t="n">
+      <c r="B173">
         <v>0.02242152466367719</v>
       </c>
-      <c r="C173" t="n">
+      <c r="C173">
         <v>-0.004024260542125346</v>
       </c>
     </row>
-    <row r="174">
-      <c r="A174" s="2" t="n">
+    <row r="174" spans="1:3">
+      <c r="A174" s="2">
         <v>45036</v>
       </c>
-      <c r="B174" t="n">
+      <c r="B174">
         <v>0.01599587203302377</v>
       </c>
-      <c r="C174" t="n">
+      <c r="C174">
         <v>0.004369039484953818</v>
       </c>
     </row>
-    <row r="175">
-      <c r="A175" s="2" t="n">
+    <row r="175" spans="1:3">
+      <c r="A175" s="2">
         <v>45035</v>
       </c>
-      <c r="B175" t="n">
+      <c r="B175">
         <v>0.02209243270695782</v>
       </c>
-      <c r="C175" t="n">
+      <c r="C175">
         <v>-0.02119382459048824</v>
       </c>
     </row>
-    <row r="176">
-      <c r="A176" s="2" t="n">
+    <row r="176" spans="1:3">
+      <c r="A176" s="2">
         <v>45034</v>
       </c>
-      <c r="B176" t="n">
+      <c r="B176">
         <v>-0.0004968944099379424</v>
       </c>
-      <c r="C176" t="n">
+      <c r="C176">
         <v>0.001386583157259258</v>
       </c>
     </row>
-    <row r="177">
-      <c r="A177" s="2" t="n">
+    <row r="177" spans="1:3">
+      <c r="A177" s="2">
         <v>45033</v>
       </c>
-      <c r="B177" t="n">
+      <c r="B177">
         <v>-0.01739995028585617</v>
       </c>
-      <c r="C177" t="n">
+      <c r="C177">
         <v>-0.002474618692309916</v>
       </c>
     </row>
-    <row r="178">
-      <c r="A178" s="2" t="n">
+    <row r="178" spans="1:3">
+      <c r="A178" s="2">
         <v>45030</v>
       </c>
-      <c r="B178" t="n">
+      <c r="B178">
         <v>0.0007589172780166908</v>
       </c>
-      <c r="C178" t="n">
+      <c r="C178">
         <v>-0.001681414266659131</v>
       </c>
     </row>
-    <row r="179">
-      <c r="A179" s="2" t="n">
+    <row r="179" spans="1:3">
+      <c r="A179" s="2">
         <v>45029</v>
       </c>
-      <c r="B179" t="n">
+      <c r="B179">
         <v>0.02022244691607678</v>
       </c>
-      <c r="C179" t="n">
+      <c r="C179">
         <v>-0.004041538029750158</v>
       </c>
     </row>
-    <row r="180">
-      <c r="A180" s="2" t="n">
+    <row r="180" spans="1:3">
+      <c r="A180" s="2">
         <v>45028</v>
       </c>
-      <c r="B180" t="n">
+      <c r="B180">
         <v>0.02155599603567881</v>
       </c>
-      <c r="C180" t="n">
+      <c r="C180">
         <v>0.00636450938670996</v>
       </c>
     </row>
-    <row r="181">
-      <c r="A181" s="2" t="n">
+    <row r="181" spans="1:3">
+      <c r="A181" s="2">
         <v>45027</v>
       </c>
-      <c r="B181" t="n">
+      <c r="B181">
         <v>0.008246422507882656</v>
       </c>
-      <c r="C181" t="n">
+      <c r="C181">
         <v>0.04287804255402716</v>
       </c>
     </row>
-    <row r="182">
-      <c r="A182" s="2" t="n">
+    <row r="182" spans="1:3">
+      <c r="A182" s="2">
         <v>45026</v>
       </c>
-      <c r="B182" t="n">
+      <c r="B182">
         <v>-0.03295645898484478</v>
       </c>
-      <c r="C182" t="n">
+      <c r="C182">
         <v>0.01016643192953914</v>
       </c>
     </row>
-    <row r="183">
-      <c r="A183" s="2" t="n">
+    <row r="183" spans="1:3">
+      <c r="A183" s="2">
         <v>45022</v>
       </c>
-      <c r="B183" t="n">
+      <c r="B183">
         <v>-0.01890547263681608</v>
       </c>
-      <c r="C183" t="n">
+      <c r="C183">
         <v>-0.001544890966349133</v>
       </c>
     </row>
-    <row r="184">
-      <c r="A184" s="2" t="n">
+    <row r="184" spans="1:3">
+      <c r="A184" s="2">
         <v>45021</v>
       </c>
-      <c r="B184" t="n">
+      <c r="B184">
         <v>0.01521298174442198</v>
       </c>
-      <c r="C184" t="n">
+      <c r="C184">
         <v>-0.008746527402840876</v>
       </c>
     </row>
-    <row r="185">
-      <c r="A185" s="2" t="n">
+    <row r="185" spans="1:3">
+      <c r="A185" s="2">
         <v>45020</v>
       </c>
-      <c r="B185" t="n">
+      <c r="B185">
         <v>0.03346653346653361</v>
       </c>
-      <c r="C185" t="n">
+      <c r="C185">
         <v>0.003576143282170596</v>
       </c>
     </row>
-    <row r="186">
-      <c r="A186" s="2" t="n">
+    <row r="186" spans="1:3">
+      <c r="A186" s="2">
         <v>45019</v>
       </c>
-      <c r="B186" t="n">
+      <c r="B186">
         <v>0.009183180280328607</v>
       </c>
-      <c r="C186" t="n">
+      <c r="C186">
         <v>-0.003690543962623472</v>
       </c>
     </row>
-    <row r="187">
-      <c r="A187" s="2" t="n">
+    <row r="187" spans="1:3">
+      <c r="A187" s="2">
         <v>45016</v>
       </c>
-      <c r="B187" t="n">
+      <c r="B187">
         <v>-0.02658045977011492</v>
       </c>
-      <c r="C187" t="n">
+      <c r="C187">
         <v>-0.01765448882975129</v>
       </c>
     </row>
-    <row r="188">
-      <c r="A188" s="2" t="n">
+    <row r="188" spans="1:3">
+      <c r="A188" s="2">
         <v>45015</v>
       </c>
-      <c r="B188" t="n">
+      <c r="B188">
         <v>0.03468634686346883</v>
       </c>
-      <c r="C188" t="n">
+      <c r="C188">
         <v>0.01886180778639002</v>
       </c>
     </row>
-    <row r="189">
-      <c r="A189" s="2" t="n">
+    <row r="189" spans="1:3">
+      <c r="A189" s="2">
         <v>45014</v>
       </c>
-      <c r="B189" t="n">
+      <c r="B189">
         <v>0.0004755111745124996</v>
       </c>
-      <c r="C189" t="n">
+      <c r="C189">
         <v>0.006008795770124031</v>
       </c>
     </row>
-    <row r="190">
-      <c r="A190" s="2" t="n">
+    <row r="190" spans="1:3">
+      <c r="A190" s="2">
         <v>45013</v>
       </c>
-      <c r="B190" t="n">
+      <c r="B190">
         <v>-0.01829847908745241</v>
       </c>
-      <c r="C190" t="n">
+      <c r="C190">
         <v>0.01520016052974826</v>
       </c>
     </row>
-    <row r="191">
-      <c r="A191" s="2" t="n">
+    <row r="191" spans="1:3">
+      <c r="A191" s="2">
         <v>45012</v>
       </c>
-      <c r="B191" t="n">
+      <c r="B191">
         <v>-0.006778019849915329</v>
       </c>
-      <c r="C191" t="n">
+      <c r="C191">
         <v>0.008509647977820167</v>
       </c>
     </row>
-    <row r="192">
-      <c r="A192" s="2" t="n">
+    <row r="192" spans="1:3">
+      <c r="A192" s="2">
         <v>45009</v>
       </c>
-      <c r="B192" t="n">
+      <c r="B192">
         <v>0.01511089446746272</v>
       </c>
-      <c r="C192" t="n">
+      <c r="C192">
         <v>0.009221248697996343</v>
       </c>
     </row>
-    <row r="193">
-      <c r="A193" s="2" t="n">
+    <row r="193" spans="1:3">
+      <c r="A193" s="2">
         <v>45008</v>
       </c>
-      <c r="B193" t="n">
+      <c r="B193">
         <v>-0.009123649459783834</v>
       </c>
-      <c r="C193" t="n">
+      <c r="C193">
         <v>-0.02289939234292215</v>
       </c>
     </row>
-    <row r="194">
-      <c r="A194" s="2" t="n">
+    <row r="194" spans="1:3">
+      <c r="A194" s="2">
         <v>45007</v>
       </c>
-      <c r="B194" t="n">
+      <c r="B194">
         <v>0.01526532590259255</v>
       </c>
-      <c r="C194" t="n">
+      <c r="C194">
         <v>-0.007693221647953385</v>
       </c>
     </row>
-    <row r="195">
-      <c r="A195" s="2" t="n">
+    <row r="195" spans="1:3">
+      <c r="A195" s="2">
         <v>45006</v>
       </c>
-      <c r="B195" t="n">
+      <c r="B195">
         <v>0.001670644391408072</v>
       </c>
-      <c r="C195" t="n">
+      <c r="C195">
         <v>0.0007431408103206749</v>
       </c>
     </row>
-    <row r="196">
-      <c r="A196" s="2" t="n">
+    <row r="196" spans="1:3">
+      <c r="A196" s="2">
         <v>45005</v>
       </c>
-      <c r="B196" t="n">
+      <c r="B196">
         <v>0.006433166547534119</v>
       </c>
-      <c r="C196" t="n">
+      <c r="C196">
         <v>-0.01038418544449016</v>
       </c>
     </row>
-    <row r="197">
-      <c r="A197" s="2" t="n">
+    <row r="197" spans="1:3">
+      <c r="A197" s="2">
         <v>45002</v>
       </c>
-      <c r="B197" t="n">
+      <c r="B197">
         <v>0.008285984848484862</v>
       </c>
-      <c r="C197" t="n">
+      <c r="C197">
         <v>-0.01404746942524293</v>
       </c>
     </row>
-    <row r="198">
-      <c r="A198" s="2" t="n">
+    <row r="198" spans="1:3">
+      <c r="A198" s="2">
         <v>45001</v>
       </c>
-      <c r="B198" t="n">
+      <c r="B198">
         <v>0.00915707912655539</v>
       </c>
-      <c r="C198" t="n">
+      <c r="C198">
         <v>0.007401996591185789</v>
       </c>
     </row>
-    <row r="199">
-      <c r="A199" s="2" t="n">
+    <row r="199" spans="1:3">
+      <c r="A199" s="2">
         <v>45000</v>
       </c>
-      <c r="B199" t="n">
+      <c r="B199">
         <v>0.005351326198231865</v>
       </c>
-      <c r="C199" t="n">
+      <c r="C199">
         <v>-0.002496793999922309</v>
       </c>
     </row>
-    <row r="200">
-      <c r="A200" s="2" t="n">
+    <row r="200" spans="1:3">
+      <c r="A200" s="2">
         <v>44999</v>
       </c>
-      <c r="B200" t="n">
+      <c r="B200">
         <v>0.01689423744503582</v>
       </c>
-      <c r="C200" t="n">
+      <c r="C200">
         <v>-0.001832798363088028</v>
       </c>
     </row>
-    <row r="201">
-      <c r="A201" s="2" t="n">
+    <row r="201" spans="1:3">
+      <c r="A201" s="2">
         <v>44998</v>
       </c>
-      <c r="B201" t="n">
+      <c r="B201">
         <v>-0.008648156577150568</v>
       </c>
-      <c r="C201" t="n">
+      <c r="C201">
         <v>-0.004796463934837569</v>
       </c>
     </row>
-    <row r="202">
-      <c r="A202" s="2" t="n">
+    <row r="202" spans="1:3">
+      <c r="A202" s="2">
         <v>44995</v>
       </c>
-      <c r="B202" t="n">
+      <c r="B202">
         <v>0.01101928374655636</v>
       </c>
-      <c r="C202" t="n">
+      <c r="C202">
         <v>-0.01382874437285264</v>
       </c>
     </row>
-    <row r="203">
-      <c r="A203" s="2" t="n">
+    <row r="203" spans="1:3">
+      <c r="A203" s="2">
         <v>44994</v>
       </c>
-      <c r="B203" t="n">
+      <c r="B203">
         <v>0.03110808356039962</v>
       </c>
-      <c r="C203" t="n">
+      <c r="C203">
         <v>-0.01378824854514737</v>
       </c>
     </row>
-    <row r="204">
-      <c r="A204" s="2" t="n">
+    <row r="204" spans="1:3">
+      <c r="A204" s="2">
         <v>44993</v>
       </c>
-      <c r="B204" t="n">
+      <c r="B204">
         <v>0.02070028628055498</v>
       </c>
-      <c r="C204" t="n">
+      <c r="C204">
         <v>0.02218213915646472</v>
       </c>
     </row>
-    <row r="205">
-      <c r="A205" s="2" t="n">
+    <row r="205" spans="1:3">
+      <c r="A205" s="2">
         <v>44992</v>
       </c>
-      <c r="B205" t="n">
+      <c r="B205">
         <v>0.006688241639697834</v>
       </c>
-      <c r="C205" t="n">
+      <c r="C205">
         <v>-0.004508118433619868</v>
       </c>
     </row>
-    <row r="206">
-      <c r="A206" s="2" t="n">
+    <row r="206" spans="1:3">
+      <c r="A206" s="2">
         <v>44991</v>
       </c>
-      <c r="B206" t="n">
+      <c r="B206">
         <v>0.0006429489927133325</v>
       </c>
-      <c r="C206" t="n">
+      <c r="C206">
         <v>0.00802957656981107</v>
       </c>
     </row>
-    <row r="207">
-      <c r="A207" s="2" t="n">
+    <row r="207" spans="1:3">
+      <c r="A207" s="2">
         <v>44988</v>
       </c>
-      <c r="B207" t="n">
+      <c r="B207">
         <v>0.008781323623902493</v>
       </c>
-      <c r="C207" t="n">
+      <c r="C207">
         <v>0.005226177341617788</v>
       </c>
     </row>
-    <row r="208">
-      <c r="A208" s="2" t="n">
+    <row r="208" spans="1:3">
+      <c r="A208" s="2">
         <v>44987</v>
       </c>
-      <c r="B208" t="n">
+      <c r="B208">
         <v>-0.03121019108280254</v>
       </c>
-      <c r="C208" t="n">
+      <c r="C208">
         <v>-0.01014513579537291</v>
       </c>
     </row>
-    <row r="209">
-      <c r="A209" s="2" t="n">
+    <row r="209" spans="1:3">
+      <c r="A209" s="2">
         <v>44986</v>
       </c>
-      <c r="B209" t="n">
+      <c r="B209">
         <v>0.001534078457155363</v>
       </c>
-      <c r="C209" t="n">
+      <c r="C209">
         <v>-0.00521289978271644</v>
       </c>
     </row>
-    <row r="210">
-      <c r="A210" s="2" t="n">
+    <row r="210" spans="1:3">
+      <c r="A210" s="2">
         <v>44985</v>
       </c>
-      <c r="B210" t="n">
+      <c r="B210">
         <v>0.02078774617067825</v>
       </c>
-      <c r="C210" t="n">
+      <c r="C210">
         <v>-0.007369147960004208</v>
       </c>
     </row>
-    <row r="211">
-      <c r="A211" s="2" t="n">
+    <row r="211" spans="1:3">
+      <c r="A211" s="2">
         <v>44984</v>
       </c>
-      <c r="B211" t="n">
+      <c r="B211">
         <v>-0.02936763129689168</v>
       </c>
-      <c r="C211" t="n">
+      <c r="C211">
         <v>-0.001530135161939339</v>
       </c>
     </row>
-    <row r="212">
-      <c r="A212" s="2" t="n">
+    <row r="212" spans="1:3">
+      <c r="A212" s="2">
         <v>44981</v>
       </c>
-      <c r="B212" t="n">
+      <c r="B212">
         <v>-0.004196113074204866</v>
       </c>
-      <c r="C212" t="n">
+      <c r="C212">
         <v>-0.01714630523579652</v>
       </c>
     </row>
-    <row r="213">
-      <c r="A213" s="2" t="n">
+    <row r="213" spans="1:3">
+      <c r="A213" s="2">
         <v>44980</v>
       </c>
-      <c r="B213" t="n">
+      <c r="B213">
         <v>0</v>
       </c>
-      <c r="C213" t="n">
+      <c r="C213">
         <v>0.005300880991488732</v>
       </c>
     </row>
-    <row r="214">
-      <c r="A214" s="2" t="n">
+    <row r="214" spans="1:3">
+      <c r="A214" s="2">
         <v>44979</v>
       </c>
-      <c r="B214" t="n">
+      <c r="B214">
         <v>-0.002439565313816949</v>
       </c>
-      <c r="C214" t="n">
+      <c r="C214">
         <v>-0.01967924027702805</v>
       </c>
     </row>
-    <row r="215">
-      <c r="A215" s="2" t="n">
+    <row r="215" spans="1:3">
+      <c r="A215" s="2">
         <v>44974</v>
       </c>
-      <c r="B215" t="n">
+      <c r="B215">
         <v>0.02000889284126295</v>
       </c>
-      <c r="C215" t="n">
+      <c r="C215">
         <v>-0.005477457804467512</v>
       </c>
     </row>
-    <row r="216">
-      <c r="A216" s="2" t="n">
+    <row r="216" spans="1:3">
+      <c r="A216" s="2">
         <v>44973</v>
       </c>
-      <c r="B216" t="n">
+      <c r="B216">
         <v>0.01721883173496064</v>
       </c>
-      <c r="C216" t="n">
+      <c r="C216">
         <v>0.004230551342263578</v>
       </c>
     </row>
-    <row r="217">
-      <c r="A217" s="2" t="n">
+    <row r="217" spans="1:3">
+      <c r="A217" s="2">
         <v>44972</v>
       </c>
-      <c r="B217" t="n">
+      <c r="B217">
         <v>0.008785086779515616</v>
       </c>
-      <c r="C217" t="n">
+      <c r="C217">
         <v>0.01656155082250432</v>
       </c>
     </row>
-    <row r="218">
-      <c r="A218" s="2" t="n">
+    <row r="218" spans="1:3">
+      <c r="A218" s="2">
         <v>44971</v>
       </c>
-      <c r="B218" t="n">
+      <c r="B218">
         <v>-0.02570093457943923</v>
       </c>
-      <c r="C218" t="n">
+      <c r="C218">
         <v>-0.01090531576723075</v>
       </c>
     </row>
-    <row r="219">
-      <c r="A219" s="2" t="n">
+    <row r="219" spans="1:3">
+      <c r="A219" s="2">
         <v>44970</v>
       </c>
-      <c r="B219" t="n">
+      <c r="B219">
         <v>-0.00501417048179631</v>
       </c>
-      <c r="C219" t="n">
+      <c r="C219">
         <v>0.00643550624133149</v>
       </c>
     </row>
-    <row r="220">
-      <c r="A220" s="2" t="n">
+    <row r="220" spans="1:3">
+      <c r="A220" s="2">
         <v>44967</v>
       </c>
-      <c r="B220" t="n">
+      <c r="B220">
         <v>-0.006573181419807117</v>
       </c>
-      <c r="C220" t="n">
+      <c r="C220">
         <v>0.003404989655140467</v>
       </c>
     </row>
-    <row r="221">
-      <c r="A221" s="2" t="n">
+    <row r="221" spans="1:3">
+      <c r="A221" s="2">
         <v>44966</v>
       </c>
-      <c r="B221" t="n">
+      <c r="B221">
         <v>-0.002205558006175612</v>
       </c>
-      <c r="C221" t="n">
+      <c r="C221">
         <v>-0.01910230975045957</v>
       </c>
     </row>
-    <row r="222">
-      <c r="A222" s="2" t="n">
+    <row r="222" spans="1:3">
+      <c r="A222" s="2">
         <v>44965</v>
       </c>
-      <c r="B222" t="n">
+      <c r="B222">
         <v>-0.007515473032714493</v>
       </c>
-      <c r="C222" t="n">
+      <c r="C222">
         <v>0.01818013343217206</v>
       </c>
     </row>
-    <row r="223">
-      <c r="A223" s="2" t="n">
+    <row r="223" spans="1:3">
+      <c r="A223" s="2">
         <v>44964</v>
       </c>
-      <c r="B223" t="n">
+      <c r="B223">
         <v>0.00222717149220486</v>
       </c>
-      <c r="C223" t="n">
+      <c r="C223">
         <v>-0.004942096333997226</v>
       </c>
     </row>
-    <row r="224">
-      <c r="A224" s="2" t="n">
+    <row r="224" spans="1:3">
+      <c r="A224" s="2">
         <v>44963</v>
       </c>
-      <c r="B224" t="n">
+      <c r="B224">
         <v>-0.002000000000000113</v>
       </c>
-      <c r="C224" t="n">
+      <c r="C224">
         <v>-0.000313392939441437</v>
       </c>
     </row>
-    <row r="225">
-      <c r="A225" s="2" t="n">
+    <row r="225" spans="1:3">
+      <c r="A225" s="2">
         <v>44960</v>
       </c>
-      <c r="B225" t="n">
+      <c r="B225">
         <v>0.007570696949454447</v>
       </c>
-      <c r="C225" t="n">
+      <c r="C225">
         <v>-0.01314413062264064</v>
       </c>
     </row>
-    <row r="226">
-      <c r="A226" s="2" t="n">
+    <row r="226" spans="1:3">
+      <c r="A226" s="2">
         <v>44959</v>
       </c>
-      <c r="B226" t="n">
+      <c r="B226">
         <v>-0.02784530386740325</v>
       </c>
-      <c r="C226" t="n">
+      <c r="C226">
         <v>-0.02108581248942598</v>
       </c>
     </row>
-    <row r="227">
-      <c r="A227" s="2" t="n">
+    <row r="227" spans="1:3">
+      <c r="A227" s="2">
         <v>44958</v>
       </c>
-      <c r="B227" t="n">
+      <c r="B227">
         <v>0.03841782223232548</v>
       </c>
-      <c r="C227" t="n">
+      <c r="C227">
         <v>-0.01082514181023853</v>
       </c>
     </row>
-    <row r="228">
-      <c r="A228" s="2" t="n">
+    <row r="228" spans="1:3">
+      <c r="A228" s="2">
         <v>44957</v>
       </c>
-      <c r="B228" t="n">
+      <c r="B228">
         <v>-0.008318739054290814</v>
       </c>
-      <c r="C228" t="n">
+      <c r="C228">
         <v>0.01469326469326471</v>
       </c>
     </row>
-    <row r="229">
-      <c r="A229" s="2" t="n">
+    <row r="229" spans="1:3">
+      <c r="A229" s="2">
         <v>44956</v>
       </c>
-      <c r="B229" t="n">
+      <c r="B229">
         <v>-0.001766004415010958</v>
       </c>
-      <c r="C229" t="n">
+      <c r="C229">
         <v>-0.005457680752342209</v>
       </c>
     </row>
-    <row r="230">
-      <c r="A230" s="2" t="n">
+    <row r="230" spans="1:3">
+      <c r="A230" s="2">
         <v>44953</v>
       </c>
-      <c r="B230" t="n">
+      <c r="B230">
         <v>-0.02587350729765592</v>
       </c>
-      <c r="C230" t="n">
+      <c r="C230">
         <v>-0.01408302587876509</v>
       </c>
     </row>
-    <row r="231">
-      <c r="A231" s="2" t="n">
+    <row r="231" spans="1:3">
+      <c r="A231" s="2">
         <v>44952</v>
       </c>
-      <c r="B231" t="n">
+      <c r="B231">
         <v>0.007037457434733385</v>
       </c>
-      <c r="C231" t="n">
+      <c r="C231">
         <v>-0.000753097771356015</v>
       </c>
     </row>
-    <row r="232">
-      <c r="A232" s="2" t="n">
+    <row r="232" spans="1:3">
+      <c r="A232" s="2">
         <v>44951</v>
       </c>
-      <c r="B232" t="n">
+      <c r="B232">
         <v>0.03020739404869266</v>
       </c>
-      <c r="C232" t="n">
+      <c r="C232">
         <v>0.01032487525214987</v>
       </c>
     </row>
-    <row r="233">
-      <c r="A233" s="2" t="n">
+    <row r="233" spans="1:3">
+      <c r="A233" s="2">
         <v>44950</v>
       </c>
-      <c r="B233" t="n">
+      <c r="B233">
         <v>0.01575492341356677</v>
       </c>
-      <c r="C233" t="n">
+      <c r="C233">
         <v>0.01180746403602217</v>
       </c>
     </row>
-    <row r="234">
-      <c r="A234" s="2" t="n">
+    <row r="234" spans="1:3">
+      <c r="A234" s="2">
         <v>44949</v>
       </c>
-      <c r="B234" t="n">
+      <c r="B234">
         <v>-0.01120206807410606</v>
       </c>
-      <c r="C234" t="n">
+      <c r="C234">
         <v>-0.005271547003143362</v>
       </c>
     </row>
-    <row r="235">
-      <c r="A235" s="2" t="n">
+    <row r="235" spans="1:3">
+      <c r="A235" s="2">
         <v>44946</v>
       </c>
-      <c r="B235" t="n">
+      <c r="B235">
         <v>0.003485838779956563</v>
       </c>
-      <c r="C235" t="n">
+      <c r="C235">
         <v>-0.006238606799638946</v>
       </c>
     </row>
-    <row r="236">
-      <c r="A236" s="2" t="n">
+    <row r="236" spans="1:3">
+      <c r="A236" s="2">
         <v>44945</v>
       </c>
-      <c r="B236" t="n">
+      <c r="B236">
         <v>0.04667824576639168</v>
       </c>
-      <c r="C236" t="n">
+      <c r="C236">
         <v>0.004926546437591162</v>
       </c>
     </row>
-    <row r="237">
-      <c r="A237" s="2" t="n">
+    <row r="237" spans="1:3">
+      <c r="A237" s="2">
         <v>44944</v>
       </c>
-      <c r="B237" t="n">
+      <c r="B237">
         <v>0.01057871810827615</v>
       </c>
-      <c r="C237" t="n">
+      <c r="C237">
         <v>0.009090174893888081</v>
       </c>
     </row>
-    <row r="238">
-      <c r="A238" s="2" t="n">
+    <row r="238" spans="1:3">
+      <c r="A238" s="2">
         <v>44943</v>
       </c>
-      <c r="B238" t="n">
+      <c r="B238">
         <v>0.02729885057471271</v>
       </c>
-      <c r="C238" t="n">
+      <c r="C238">
         <v>0.02038218893355181</v>
       </c>
     </row>
-    <row r="239">
-      <c r="A239" s="2" t="n">
+    <row r="239" spans="1:3">
+      <c r="A239" s="2">
         <v>44942</v>
       </c>
-      <c r="B239" t="n">
+      <c r="B239">
         <v>-0.01198801198801192</v>
       </c>
-      <c r="C239" t="n">
+      <c r="C239">
         <v>-0.01535396155649316</v>
       </c>
     </row>
-    <row r="240">
-      <c r="A240" s="2" t="n">
+    <row r="240" spans="1:3">
+      <c r="A240" s="2">
         <v>44939</v>
       </c>
-      <c r="B240" t="n">
+      <c r="B240">
         <v>-0.003640040444893855</v>
       </c>
-      <c r="C240" t="n">
+      <c r="C240">
         <v>-0.008589790573576339</v>
       </c>
     </row>
-    <row r="241">
-      <c r="A241" s="2" t="n">
+    <row r="241" spans="1:3">
+      <c r="A241" s="2">
         <v>44938</v>
       </c>
-      <c r="B241" t="n">
+      <c r="B241">
         <v>-0.003247412218388535</v>
       </c>
-      <c r="C241" t="n">
+      <c r="C241">
         <v>0.001020015568658605</v>
       </c>
     </row>
-    <row r="242">
-      <c r="A242" s="2" t="n">
+    <row r="242" spans="1:3">
+      <c r="A242" s="2">
         <v>44937</v>
       </c>
-      <c r="B242" t="n">
+      <c r="B242">
         <v>-0.02015882712278561</v>
       </c>
-      <c r="C242" t="n">
+      <c r="C242">
         <v>0.007672749567224413</v>
       </c>
     </row>
-    <row r="243">
-      <c r="A243" s="2" t="n">
+    <row r="243" spans="1:3">
+      <c r="A243" s="2">
         <v>44936</v>
       </c>
-      <c r="B243" t="n">
+      <c r="B243">
         <v>0.01475477971737327</v>
       </c>
-      <c r="C243" t="n">
+      <c r="C243">
         <v>0.01542658866397506</v>
       </c>
     </row>
-    <row r="244">
-      <c r="A244" s="2" t="n">
+    <row r="244" spans="1:3">
+      <c r="A244" s="2">
         <v>44935</v>
       </c>
-      <c r="B244" t="n">
+      <c r="B244">
         <v>0.01269711243088278</v>
       </c>
-      <c r="C244" t="n">
+      <c r="C244">
         <v>0.003592561284869067</v>
       </c>
     </row>
-    <row r="245">
-      <c r="A245" s="2" t="n">
+    <row r="245" spans="1:3">
+      <c r="A245" s="2">
         <v>44932</v>
       </c>
-      <c r="B245" t="n">
+      <c r="B245">
         <v>-0.01314459049545003</v>
       </c>
-      <c r="C245" t="n">
+      <c r="C245">
         <v>0.01225841254487614</v>
       </c>
     </row>
-    <row r="246">
-      <c r="A246" s="2" t="n">
+    <row r="246" spans="1:3">
+      <c r="A246" s="2">
         <v>44931</v>
       </c>
-      <c r="B246" t="n">
+      <c r="B246">
         <v>0.006352459016393475</v>
       </c>
-      <c r="C246" t="n">
+      <c r="C246">
         <v>0.02073404598705064</v>
       </c>
     </row>
-    <row r="247">
-      <c r="A247" s="2" t="n">
+    <row r="247" spans="1:3">
+      <c r="A247" s="2">
         <v>44930</v>
       </c>
-      <c r="B247" t="n">
+      <c r="B247">
         <v>-0.00610873549175317</v>
       </c>
-      <c r="C247" t="n">
+      <c r="C247">
         <v>0.01121287176237917</v>
       </c>
     </row>
-    <row r="248">
-      <c r="A248" s="2" t="n">
+    <row r="248" spans="1:3">
+      <c r="A248" s="2">
         <v>44929</v>
       </c>
-      <c r="B248" t="n">
+      <c r="B248">
         <v>-0.002048760499897551</v>
       </c>
-      <c r="C248" t="n">
+      <c r="C248">
         <v>-0.02077536286380388</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="25.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Beta</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>-0.1794044374275717</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>